<commit_message>
Always a zero in one range in levels.
</commit_message>
<xml_diff>
--- a/WindDataProcessing/TestovaciData/Levels.xlsx
+++ b/WindDataProcessing/TestovaciData/Levels.xlsx
@@ -1867,16 +1867,16 @@
     </row>
     <row r="31">
       <c r="B31" s="0">
-        <v>552.961111111088</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0">
-        <v>-4446.250694444468</v>
+        <v>-4722.7312500000035</v>
       </c>
       <c r="D31" s="0">
-        <v>-9445.462500000023</v>
+        <v>-9445.462500000007</v>
       </c>
       <c r="E31" s="0">
-        <v>0.0009299679173655337</v>
+        <v>0.000896718815091295</v>
       </c>
       <c r="H31" s="0">
         <v>-42992.118888888894</v>
@@ -1929,16 +1929,16 @@
     </row>
     <row r="32">
       <c r="B32" s="0">
-        <v>10551.384722222212</v>
+        <v>10003.19051724138</v>
       </c>
       <c r="C32" s="0">
-        <v>5552.172916666656</v>
+        <v>5001.59525862069</v>
       </c>
       <c r="D32" s="0">
-        <v>552.9611111111008</v>
+        <v>0</v>
       </c>
       <c r="E32" s="0">
-        <v>0.0009470330075146553</v>
+        <v>0.000880534802966178</v>
       </c>
       <c r="H32" s="0">
         <v>-42140.86527777778</v>
@@ -1991,13 +1991,13 @@
     </row>
     <row r="33">
       <c r="B33" s="0">
-        <v>20549.808333333334</v>
+        <v>20006.38103448276</v>
       </c>
       <c r="C33" s="0">
-        <v>15550.59652777778</v>
+        <v>15004.78577586207</v>
       </c>
       <c r="D33" s="0">
-        <v>10551.384722222225</v>
+        <v>10003.19051724138</v>
       </c>
       <c r="E33" s="0">
         <v>0.0015288293631692575</v>
@@ -2053,16 +2053,16 @@
     </row>
     <row r="34">
       <c r="B34" s="0">
-        <v>30548.2319444444</v>
+        <v>30009.57155172414</v>
       </c>
       <c r="C34" s="0">
-        <v>25549.020138888845</v>
+        <v>25007.976293103453</v>
       </c>
       <c r="D34" s="0">
-        <v>20549.80833333329</v>
+        <v>20006.38103448276</v>
       </c>
       <c r="E34" s="0">
-        <v>0.0015613232557086356</v>
+        <v>0.0015447616387160878</v>
       </c>
       <c r="H34" s="0">
         <v>-40438.35805555556</v>
@@ -2115,16 +2115,16 @@
     </row>
     <row r="35">
       <c r="B35" s="0">
-        <v>40546.655555555524</v>
+        <v>40012.76206896552</v>
       </c>
       <c r="C35" s="0">
-        <v>35547.44374999997</v>
+        <v>35011.16681034483</v>
       </c>
       <c r="D35" s="0">
-        <v>30548.231944444415</v>
+        <v>30009.57155172414</v>
       </c>
       <c r="E35" s="0">
-        <v>0.002076117933658189</v>
+        <v>0.00209280541893988</v>
       </c>
       <c r="H35" s="0">
         <v>-39587.10444444445</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="36">
       <c r="B36" s="0">
-        <v>50545.07916666665</v>
+        <v>50015.952586206906</v>
       </c>
       <c r="C36" s="0">
-        <v>45545.86736111109</v>
+        <v>45014.357327586215</v>
       </c>
       <c r="D36" s="0">
-        <v>40546.65555555554</v>
+        <v>40012.76206896552</v>
       </c>
       <c r="E36" s="0">
-        <v>0.0021258027846358324</v>
+        <v>0.0019929322438280214</v>
       </c>
       <c r="H36" s="0">
         <v>-38735.85083333334</v>
@@ -2239,16 +2239,16 @@
     </row>
     <row r="37">
       <c r="B37" s="0">
-        <v>60543.50277777777</v>
+        <v>60019.14310344829</v>
       </c>
       <c r="C37" s="0">
-        <v>55544.29097222222</v>
+        <v>55017.5478448276</v>
       </c>
       <c r="D37" s="0">
-        <v>50545.07916666666</v>
+        <v>50015.952586206906</v>
       </c>
       <c r="E37" s="0">
-        <v>0.002508104526645004</v>
+        <v>0.002707347403712149</v>
       </c>
       <c r="H37" s="0">
         <v>-37884.597222222226</v>
@@ -2301,16 +2301,16 @@
     </row>
     <row r="38">
       <c r="B38" s="0">
-        <v>70541.9263888889</v>
+        <v>70022.33362068966</v>
       </c>
       <c r="C38" s="0">
-        <v>65542.71458333335</v>
+        <v>65020.73836206897</v>
       </c>
       <c r="D38" s="0">
-        <v>60543.50277777779</v>
+        <v>60019.14310344828</v>
       </c>
       <c r="E38" s="0">
-        <v>0.0032225196865291314</v>
+        <v>0.0030730875287287725</v>
       </c>
       <c r="H38" s="0">
         <v>-37033.343611111115</v>
@@ -2363,16 +2363,16 @@
     </row>
     <row r="39">
       <c r="B39" s="0">
-        <v>80540.34999999996</v>
+        <v>80025.52413793105</v>
       </c>
       <c r="C39" s="0">
-        <v>75541.13819444441</v>
+        <v>75023.92887931035</v>
       </c>
       <c r="D39" s="0">
-        <v>70541.92638888885</v>
+        <v>70022.33362068966</v>
       </c>
       <c r="E39" s="0">
-        <v>0.008055669874877101</v>
+        <v>0.007607247533186884</v>
       </c>
       <c r="H39" s="0">
         <v>-36182.090000000004</v>
@@ -2425,16 +2425,16 @@
     </row>
     <row r="40">
       <c r="B40" s="0">
-        <v>90538.77361111109</v>
+        <v>90028.71465517243</v>
       </c>
       <c r="C40" s="0">
-        <v>85539.56180555554</v>
+        <v>85027.11939655173</v>
       </c>
       <c r="D40" s="0">
-        <v>80540.34999999998</v>
+        <v>80025.52413793105</v>
       </c>
       <c r="E40" s="0">
-        <v>0.02037598262392247</v>
+        <v>0.01961200848134984</v>
       </c>
       <c r="H40" s="0">
         <v>-35330.83638888889</v>
@@ -2487,16 +2487,16 @@
     </row>
     <row r="41">
       <c r="B41" s="0">
-        <v>100537.19722222221</v>
+        <v>100031.90517241381</v>
       </c>
       <c r="C41" s="0">
-        <v>95537.98541666666</v>
+        <v>95030.30991379311</v>
       </c>
       <c r="D41" s="0">
-        <v>90538.7736111111</v>
+        <v>90028.71465517243</v>
       </c>
       <c r="E41" s="0">
-        <v>0.03360270604632324</v>
+        <v>0.033054158792942906</v>
       </c>
       <c r="H41" s="0">
         <v>-34479.58277777778</v>
@@ -2549,16 +2549,16 @@
     </row>
     <row r="42">
       <c r="B42" s="0">
-        <v>110535.62083333333</v>
+        <v>110035.0956896552</v>
       </c>
       <c r="C42" s="0">
-        <v>105536.40902777779</v>
+        <v>105033.5004310345</v>
       </c>
       <c r="D42" s="0">
-        <v>100537.19722222222</v>
+        <v>100031.90517241381</v>
       </c>
       <c r="E42" s="0">
-        <v>0.044241789432633266</v>
+        <v>0.0433937485222065</v>
       </c>
       <c r="H42" s="0">
         <v>-33628.32916666667</v>
@@ -2611,16 +2611,16 @@
     </row>
     <row r="43">
       <c r="B43" s="0">
-        <v>120534.0444444444</v>
+        <v>120038.28620689658</v>
       </c>
       <c r="C43" s="0">
-        <v>115534.83263888885</v>
+        <v>115036.69094827588</v>
       </c>
       <c r="D43" s="0">
-        <v>110535.62083333329</v>
+        <v>110035.0956896552</v>
       </c>
       <c r="E43" s="0">
-        <v>0.06417984978003824</v>
+        <v>0.0630993168902699</v>
       </c>
       <c r="H43" s="0">
         <v>-32777.07555555556</v>
@@ -2673,16 +2673,16 @@
     </row>
     <row r="44">
       <c r="B44" s="0">
-        <v>130532.46805555552</v>
+        <v>130041.47672413794</v>
       </c>
       <c r="C44" s="0">
-        <v>125533.25624999998</v>
+        <v>125039.88146551725</v>
       </c>
       <c r="D44" s="0">
-        <v>120534.04444444441</v>
+        <v>120038.28620689656</v>
       </c>
       <c r="E44" s="0">
-        <v>0.06218691753621007</v>
+        <v>0.06295152102022847</v>
       </c>
       <c r="H44" s="0">
         <v>-31925.821944444448</v>
@@ -2735,16 +2735,16 @@
     </row>
     <row r="45">
       <c r="B45" s="0">
-        <v>140530.89166666666</v>
+        <v>140044.66724137933</v>
       </c>
       <c r="C45" s="0">
-        <v>135531.6798611111</v>
+        <v>135043.07198275864</v>
       </c>
       <c r="D45" s="0">
-        <v>130532.46805555554</v>
+        <v>130041.47672413794</v>
       </c>
       <c r="E45" s="0">
-        <v>0.06898465972938934</v>
+        <v>0.06930058913513923</v>
       </c>
       <c r="H45" s="0">
         <v>-31074.568333333336</v>
@@ -2797,16 +2797,16 @@
     </row>
     <row r="46">
       <c r="B46" s="0">
-        <v>150529.3152777778</v>
+        <v>150047.8577586207</v>
       </c>
       <c r="C46" s="0">
-        <v>145530.10347222222</v>
+        <v>145046.2625</v>
       </c>
       <c r="D46" s="0">
-        <v>140530.89166666666</v>
+        <v>140044.66724137933</v>
       </c>
       <c r="E46" s="0">
-        <v>0.054929298987029425</v>
+        <v>0.0553782248018762</v>
       </c>
       <c r="H46" s="0">
         <v>-30223.314722222225</v>
@@ -2859,16 +2859,16 @@
     </row>
     <row r="47">
       <c r="B47" s="0">
-        <v>160527.7388888889</v>
+        <v>160051.0482758621</v>
       </c>
       <c r="C47" s="0">
-        <v>155528.52708333335</v>
+        <v>155049.4530172414</v>
       </c>
       <c r="D47" s="0">
-        <v>150529.3152777778</v>
+        <v>150047.85775862072</v>
       </c>
       <c r="E47" s="0">
-        <v>0.03380476008800234</v>
+        <v>0.03486860549248876</v>
       </c>
       <c r="H47" s="0">
         <v>-29372.061111111114</v>
@@ -2921,16 +2921,16 @@
     </row>
     <row r="48">
       <c r="B48" s="0">
-        <v>170526.16249999998</v>
+        <v>170054.23879310346</v>
       </c>
       <c r="C48" s="0">
-        <v>165526.95069444441</v>
+        <v>165052.64353448278</v>
       </c>
       <c r="D48" s="0">
-        <v>160527.73888888885</v>
+        <v>160051.0482758621</v>
       </c>
       <c r="E48" s="0">
-        <v>0.022755749460483726</v>
+        <v>0.023320396601487825</v>
       </c>
       <c r="H48" s="0">
         <v>-28520.807500000003</v>
@@ -2983,16 +2983,16 @@
     </row>
     <row r="49">
       <c r="B49" s="0">
-        <v>180524.5861111111</v>
+        <v>180057.42931034483</v>
       </c>
       <c r="C49" s="0">
-        <v>175525.37430555554</v>
+        <v>175055.83405172414</v>
       </c>
       <c r="D49" s="0">
-        <v>170526.16249999998</v>
+        <v>170054.23879310346</v>
       </c>
       <c r="E49" s="0">
-        <v>0.011878653512754682</v>
+        <v>0.01211080931255344</v>
       </c>
       <c r="H49" s="0">
         <v>-27669.55388888889</v>
@@ -3045,16 +3045,16 @@
     </row>
     <row r="50">
       <c r="B50" s="0">
-        <v>190523.00972222222</v>
+        <v>190060.61982758623</v>
       </c>
       <c r="C50" s="0">
-        <v>185523.79791666666</v>
+        <v>185059.02456896554</v>
       </c>
       <c r="D50" s="0">
-        <v>180524.5861111111</v>
+        <v>180057.42931034486</v>
       </c>
       <c r="E50" s="0">
-        <v>0.013058548224946185</v>
+        <v>0.012691841305089435</v>
       </c>
       <c r="H50" s="0">
         <v>-26818.30027777778</v>
@@ -3107,16 +3107,16 @@
     </row>
     <row r="51">
       <c r="B51" s="0">
-        <v>200521.43333333335</v>
+        <v>200063.8103448276</v>
       </c>
       <c r="C51" s="0">
-        <v>195522.2215277778</v>
+        <v>195062.2150862069</v>
       </c>
       <c r="D51" s="0">
-        <v>190523.00972222222</v>
+        <v>190060.61982758623</v>
       </c>
       <c r="E51" s="0">
-        <v>0.024883717117411806</v>
+        <v>0.023884982181663707</v>
       </c>
       <c r="H51" s="0">
         <v>-25967.04666666667</v>
@@ -3169,16 +3169,16 @@
     </row>
     <row r="52">
       <c r="B52" s="0">
-        <v>210519.85694444447</v>
+        <v>210067.000862069</v>
       </c>
       <c r="C52" s="0">
-        <v>205520.6451388889</v>
+        <v>205065.4056034483</v>
       </c>
       <c r="D52" s="0">
-        <v>200521.43333333335</v>
+        <v>200063.81034482762</v>
       </c>
       <c r="E52" s="0">
-        <v>0.035388213772714464</v>
+        <v>0.03537144216293139</v>
       </c>
       <c r="H52" s="0">
         <v>-25115.793055555565</v>
@@ -3231,16 +3231,16 @@
     </row>
     <row r="53">
       <c r="B53" s="0">
-        <v>220518.28055555554</v>
+        <v>220070.19137931036</v>
       </c>
       <c r="C53" s="0">
-        <v>215519.06874999998</v>
+        <v>215068.59612068968</v>
       </c>
       <c r="D53" s="0">
-        <v>210519.85694444441</v>
+        <v>210067.000862069</v>
       </c>
       <c r="E53" s="0">
-        <v>0.03493895114139917</v>
+        <v>0.03543831860927317</v>
       </c>
       <c r="H53" s="0">
         <v>-24264.539444444454</v>
@@ -3293,16 +3293,16 @@
     </row>
     <row r="54">
       <c r="B54" s="0">
-        <v>230516.70416666666</v>
+        <v>230073.38189655176</v>
       </c>
       <c r="C54" s="0">
-        <v>225517.4923611111</v>
+        <v>225071.78663793107</v>
       </c>
       <c r="D54" s="0">
-        <v>220518.28055555554</v>
+        <v>220070.1913793104</v>
       </c>
       <c r="E54" s="0">
-        <v>0.021655734433699145</v>
+        <v>0.022338329333980965</v>
       </c>
       <c r="H54" s="0">
         <v>-23413.285833333342</v>
@@ -3355,16 +3355,16 @@
     </row>
     <row r="55">
       <c r="B55" s="0">
-        <v>240515.1277777778</v>
+        <v>240076.57241379312</v>
       </c>
       <c r="C55" s="0">
-        <v>235515.91597222222</v>
+        <v>235074.97715517244</v>
       </c>
       <c r="D55" s="0">
-        <v>230516.70416666666</v>
+        <v>230073.38189655176</v>
       </c>
       <c r="E55" s="0">
-        <v>0.010253384556388025</v>
+        <v>0.010469651098279485</v>
       </c>
       <c r="H55" s="0">
         <v>-22562.03222222223</v>
@@ -3417,16 +3417,16 @@
     </row>
     <row r="56">
       <c r="B56" s="0">
-        <v>250513.5513888889</v>
+        <v>250079.7629310345</v>
       </c>
       <c r="C56" s="0">
-        <v>245514.33958333335</v>
+        <v>245078.1676724138</v>
       </c>
       <c r="D56" s="0">
-        <v>240515.1277777778</v>
+        <v>240076.57241379312</v>
       </c>
       <c r="E56" s="0">
-        <v>0.009504207327056374</v>
+        <v>0.0093377515044317</v>
       </c>
       <c r="H56" s="0">
         <v>-21710.77861111112</v>
@@ -3479,16 +3479,16 @@
     </row>
     <row r="57">
       <c r="B57" s="0">
-        <v>260511.97499999998</v>
+        <v>260082.9534482759</v>
       </c>
       <c r="C57" s="0">
-        <v>255512.76319444441</v>
+        <v>255081.3581896552</v>
       </c>
       <c r="D57" s="0">
-        <v>250513.55138888885</v>
+        <v>250079.76293103452</v>
       </c>
       <c r="E57" s="0">
-        <v>0.013931932208872712</v>
+        <v>0.013499147070048559</v>
       </c>
       <c r="H57" s="0">
         <v>-20859.52500000001</v>
@@ -3541,16 +3541,16 @@
     </row>
     <row r="58">
       <c r="B58" s="0">
-        <v>270510.3986111111</v>
+        <v>270086.1439655173</v>
       </c>
       <c r="C58" s="0">
-        <v>265511.18680555554</v>
+        <v>265084.5487068966</v>
       </c>
       <c r="D58" s="0">
-        <v>260511.97499999998</v>
+        <v>260082.9534482759</v>
       </c>
       <c r="E58" s="0">
-        <v>0.027497955725263663</v>
+        <v>0.027597829218838472</v>
       </c>
       <c r="H58" s="0">
         <v>-20008.271388888897</v>
@@ -3603,16 +3603,16 @@
     </row>
     <row r="59">
       <c r="B59" s="0">
-        <v>280508.8222222222</v>
+        <v>280089.33448275866</v>
       </c>
       <c r="C59" s="0">
-        <v>275509.61041666666</v>
+        <v>275087.739224138</v>
       </c>
       <c r="D59" s="0">
-        <v>270510.3986111111</v>
+        <v>270086.1439655173</v>
       </c>
       <c r="E59" s="0">
-        <v>0.030144729332516742</v>
+        <v>0.02987840001631725</v>
       </c>
       <c r="H59" s="0">
         <v>-19157.017777777786</v>
@@ -3665,16 +3665,16 @@
     </row>
     <row r="60">
       <c r="B60" s="0">
-        <v>290507.24583333335</v>
+        <v>290092.525</v>
       </c>
       <c r="C60" s="0">
-        <v>285508.0340277778</v>
+        <v>285090.92974137934</v>
       </c>
       <c r="D60" s="0">
-        <v>280508.8222222222</v>
+        <v>280089.33448275866</v>
       </c>
       <c r="E60" s="0">
-        <v>0.0368697966215946</v>
+        <v>0.0364703026472954</v>
       </c>
       <c r="H60" s="0">
         <v>-18305.764166666675</v>
@@ -3727,16 +3727,16 @@
     </row>
     <row r="61">
       <c r="B61" s="0">
-        <v>300505.6694444445</v>
+        <v>300095.7155172414</v>
       </c>
       <c r="C61" s="0">
-        <v>295506.4576388889</v>
+        <v>295094.1202586207</v>
       </c>
       <c r="D61" s="0">
-        <v>290507.24583333335</v>
+        <v>290092.525</v>
       </c>
       <c r="E61" s="0">
-        <v>0.05256670672262118</v>
+        <v>0.05210063041927212</v>
       </c>
       <c r="H61" s="0">
         <v>-17454.510555555564</v>
@@ -3789,16 +3789,16 @@
     </row>
     <row r="62">
       <c r="B62" s="0">
-        <v>310504.0930555556</v>
+        <v>310098.9060344828</v>
       </c>
       <c r="C62" s="0">
-        <v>305504.88125000003</v>
+        <v>305097.31077586213</v>
       </c>
       <c r="D62" s="0">
-        <v>300505.6694444445</v>
+        <v>300095.71551724145</v>
       </c>
       <c r="E62" s="0">
-        <v>0.05942468661475741</v>
+        <v>0.05935814634795824</v>
       </c>
       <c r="H62" s="0">
         <v>-16603.256944444453</v>
@@ -3851,16 +3851,16 @@
     </row>
     <row r="63">
       <c r="B63" s="0">
-        <v>320502.5166666667</v>
+        <v>320102.0965517242</v>
       </c>
       <c r="C63" s="0">
-        <v>315503.30486111116</v>
+        <v>315100.5012931035</v>
       </c>
       <c r="D63" s="0">
-        <v>310504.0930555556</v>
+        <v>310098.9060344828</v>
       </c>
       <c r="E63" s="0">
-        <v>0.04446022419553005</v>
+        <v>0.04472651144947882</v>
       </c>
       <c r="H63" s="0">
         <v>-15752.003333333341</v>
@@ -3913,16 +3913,16 @@
     </row>
     <row r="64">
       <c r="B64" s="0">
-        <v>330500.9402777777</v>
+        <v>330105.28706896555</v>
       </c>
       <c r="C64" s="0">
-        <v>325501.72847222217</v>
+        <v>325103.69181034487</v>
       </c>
       <c r="D64" s="0">
-        <v>320502.5166666666</v>
+        <v>320102.0965517242</v>
       </c>
       <c r="E64" s="0">
-        <v>0.033490869449834496</v>
+        <v>0.03409011041128329</v>
       </c>
       <c r="H64" s="0">
         <v>-14900.74972222223</v>
@@ -3975,16 +3975,16 @@
     </row>
     <row r="65">
       <c r="B65" s="0">
-        <v>340499.36388888885</v>
+        <v>340108.4775862069</v>
       </c>
       <c r="C65" s="0">
-        <v>335500.1520833333</v>
+        <v>335106.88232758624</v>
       </c>
       <c r="D65" s="0">
-        <v>330500.9402777777</v>
+        <v>330105.28706896555</v>
       </c>
       <c r="E65" s="0">
-        <v>0.01985801154935257</v>
+        <v>0.020790164156050794</v>
       </c>
       <c r="H65" s="0">
         <v>-14049.496111111119</v>
@@ -4037,16 +4037,16 @@
     </row>
     <row r="66">
       <c r="B66" s="0">
-        <v>350497.7875</v>
+        <v>350111.6681034483</v>
       </c>
       <c r="C66" s="0">
-        <v>345498.5756944444</v>
+        <v>345110.0728448276</v>
       </c>
       <c r="D66" s="0">
-        <v>340499.36388888885</v>
+        <v>340108.4775862069</v>
       </c>
       <c r="E66" s="0">
-        <v>0.008022876533217389</v>
+        <v>0.008255914684891933</v>
       </c>
       <c r="H66" s="0">
         <v>-13198.242500000008</v>
@@ -4099,16 +4099,16 @@
     </row>
     <row r="67">
       <c r="B67" s="0">
-        <v>360496.2111111111</v>
+        <v>360114.8586206897</v>
       </c>
       <c r="C67" s="0">
-        <v>355496.99930555554</v>
+        <v>355113.26336206903</v>
       </c>
       <c r="D67" s="0">
-        <v>350497.7875</v>
+        <v>350111.66810344835</v>
       </c>
       <c r="E67" s="0">
-        <v>0.00331230278045972</v>
+        <v>0.0033455939449846548</v>
       </c>
       <c r="H67" s="0">
         <v>-12346.988888888896</v>
@@ -4161,16 +4161,16 @@
     </row>
     <row r="68">
       <c r="B68" s="0">
-        <v>370494.6347222222</v>
+        <v>370118.0491379311</v>
       </c>
       <c r="C68" s="0">
-        <v>365495.42291666666</v>
+        <v>365116.4538793104</v>
       </c>
       <c r="D68" s="0">
-        <v>360496.2111111111</v>
+        <v>360114.8586206897</v>
       </c>
       <c r="E68" s="0">
-        <v>0.004527556313140459</v>
+        <v>0.00432780932599085</v>
       </c>
       <c r="H68" s="0">
         <v>-11495.735277777785</v>
@@ -4223,16 +4223,16 @@
     </row>
     <row r="69">
       <c r="B69" s="0">
-        <v>380493.05833333335</v>
+        <v>380121.23965517245</v>
       </c>
       <c r="C69" s="0">
-        <v>375493.8465277778</v>
+        <v>375119.64439655177</v>
       </c>
       <c r="D69" s="0">
-        <v>370494.6347222222</v>
+        <v>370118.0491379311</v>
       </c>
       <c r="E69" s="0">
-        <v>0.006674710397478142</v>
+        <v>0.0065082545748534676</v>
       </c>
       <c r="H69" s="0">
         <v>-10644.481666666674</v>
@@ -4285,16 +4285,16 @@
     </row>
     <row r="70">
       <c r="B70" s="0">
-        <v>390491.4819444445</v>
+        <v>390124.4301724138</v>
       </c>
       <c r="C70" s="0">
-        <v>385492.2701388889</v>
+        <v>385122.83491379314</v>
       </c>
       <c r="D70" s="0">
-        <v>380493.05833333335</v>
+        <v>380121.23965517245</v>
       </c>
       <c r="E70" s="0">
-        <v>0.005725828243247578</v>
+        <v>0.005992157559447057</v>
       </c>
       <c r="H70" s="0">
         <v>-9793.228055555563</v>
@@ -4347,13 +4347,13 @@
     </row>
     <row r="71">
       <c r="B71" s="0">
-        <v>400489.9055555556</v>
+        <v>400127.62068965525</v>
       </c>
       <c r="C71" s="0">
-        <v>395490.69375000003</v>
+        <v>395126.02543103456</v>
       </c>
       <c r="D71" s="0">
-        <v>390491.4819444445</v>
+        <v>390124.4301724139</v>
       </c>
       <c r="E71" s="0">
         <v>0.0034955302128674777</v>
@@ -4409,16 +4409,16 @@
     </row>
     <row r="72">
       <c r="B72" s="0">
-        <v>410488.3291666667</v>
+        <v>410130.8112068966</v>
       </c>
       <c r="C72" s="0">
-        <v>405489.11736111116</v>
+        <v>405129.21594827593</v>
       </c>
       <c r="D72" s="0">
-        <v>400489.9055555556</v>
+        <v>400127.62068965525</v>
       </c>
       <c r="E72" s="0">
-        <v>0.001797680822095798</v>
+        <v>0.0019974278092454085</v>
       </c>
       <c r="H72" s="0">
         <v>-8090.72083333334</v>
@@ -4471,13 +4471,13 @@
     </row>
     <row r="73">
       <c r="B73" s="0">
-        <v>420486.7527777777</v>
+        <v>420134.001724138</v>
       </c>
       <c r="C73" s="0">
-        <v>415487.54097222217</v>
+        <v>415132.4064655173</v>
       </c>
       <c r="D73" s="0">
-        <v>410488.3291666666</v>
+        <v>410130.8112068966</v>
       </c>
       <c r="E73" s="0">
         <v>0.0007155919475147914</v>
@@ -4533,13 +4533,13 @@
     </row>
     <row r="74">
       <c r="B74" s="0">
-        <v>430485.17638888885</v>
+        <v>430137.19224137935</v>
       </c>
       <c r="C74" s="0">
-        <v>425485.9645833333</v>
+        <v>425135.59698275867</v>
       </c>
       <c r="D74" s="0">
-        <v>420486.7527777777</v>
+        <v>420134.001724138</v>
       </c>
       <c r="E74" s="0">
         <v>6.654026679917368E-05</v>
@@ -4595,13 +4595,13 @@
     </row>
     <row r="75">
       <c r="B75" s="0">
-        <v>440483.6</v>
+        <v>440140.3827586207</v>
       </c>
       <c r="C75" s="0">
-        <v>435484.3881944444</v>
+        <v>435138.78750000003</v>
       </c>
       <c r="D75" s="0">
-        <v>430485.17638888885</v>
+        <v>430137.19224137935</v>
       </c>
       <c r="E75" s="0">
         <v>0.0002823026986081697</v>
@@ -4657,13 +4657,13 @@
     </row>
     <row r="76">
       <c r="B76" s="0">
-        <v>450482.0236111111</v>
+        <v>450143.57327586215</v>
       </c>
       <c r="C76" s="0">
-        <v>445482.81180555554</v>
+        <v>445141.97801724146</v>
       </c>
       <c r="D76" s="0">
-        <v>440483.6</v>
+        <v>440140.3827586208</v>
       </c>
       <c r="E76" s="0">
         <v>0.00013287054080781102</v>
@@ -4719,13 +4719,13 @@
     </row>
     <row r="77">
       <c r="B77" s="0">
-        <v>460480.4472222222</v>
+        <v>460146.7637931035</v>
       </c>
       <c r="C77" s="0">
-        <v>455481.23541666666</v>
+        <v>455145.16853448283</v>
       </c>
       <c r="D77" s="0">
-        <v>450482.0236111111</v>
+        <v>450143.57327586215</v>
       </c>
       <c r="E77" s="0">
         <v>0.00023249197934138344</v>
@@ -4781,13 +4781,13 @@
     </row>
     <row r="78">
       <c r="B78" s="0">
-        <v>470478.87083333335</v>
+        <v>470149.9543103449</v>
       </c>
       <c r="C78" s="0">
-        <v>465479.6590277778</v>
+        <v>465148.3590517242</v>
       </c>
       <c r="D78" s="0">
-        <v>460480.4472222222</v>
+        <v>460146.7637931035</v>
       </c>
       <c r="E78" s="0">
         <v>0.00013287054080781102</v>
@@ -4843,13 +4843,13 @@
     </row>
     <row r="79">
       <c r="B79" s="0">
-        <v>480477.2944444445</v>
+        <v>480153.14482758625</v>
       </c>
       <c r="C79" s="0">
-        <v>475478.0826388889</v>
+        <v>475151.54956896557</v>
       </c>
       <c r="D79" s="0">
-        <v>470478.87083333335</v>
+        <v>470149.9543103449</v>
       </c>
       <c r="E79" s="0">
         <v>0.00018268126007459722</v>
@@ -4905,13 +4905,13 @@
     </row>
     <row r="80">
       <c r="B80" s="0">
-        <v>490475.7180555556</v>
+        <v>490156.3353448276</v>
       </c>
       <c r="C80" s="0">
-        <v>485476.50625000003</v>
+        <v>485154.74008620693</v>
       </c>
       <c r="D80" s="0">
-        <v>480477.2944444445</v>
+        <v>480153.14482758625</v>
       </c>
       <c r="E80" s="0">
         <v>0.00013287054080781102</v>
@@ -4967,13 +4967,13 @@
     </row>
     <row r="81">
       <c r="B81" s="0">
-        <v>500474.1416666667</v>
+        <v>500159.52586206904</v>
       </c>
       <c r="C81" s="0">
-        <v>495474.92986111116</v>
+        <v>495157.93060344836</v>
       </c>
       <c r="D81" s="0">
-        <v>490475.7180555556</v>
+        <v>490156.3353448277</v>
       </c>
       <c r="E81" s="0">
         <v>8.305982154102482E-05</v>
@@ -5029,28 +5029,28 @@
     </row>
     <row r="82">
       <c r="B82" s="0">
-        <v>510472.5652777777</v>
+        <v>510162.7163793104</v>
       </c>
       <c r="C82" s="0">
-        <v>505473.35347222217</v>
+        <v>505161.1211206897</v>
       </c>
       <c r="D82" s="0">
-        <v>500474.1416666666</v>
+        <v>500159.52586206904</v>
       </c>
       <c r="E82" s="0">
         <v>0.00013287054080781102</v>
       </c>
       <c r="H82" s="0">
-        <v>421.81527777777205</v>
+        <v>0</v>
       </c>
       <c r="I82" s="0">
-        <v>-3.8115277777834535</v>
+        <v>-214.7191666666696</v>
       </c>
       <c r="J82" s="0">
-        <v>-429.43833333333896</v>
+        <v>-429.4383333333392</v>
       </c>
       <c r="K82" s="0">
-        <v>0.05116385215680796</v>
+        <v>0.026572191084759444</v>
       </c>
       <c r="N82" s="0">
         <v>-1183243.5631944444</v>
@@ -5091,28 +5091,28 @@
     </row>
     <row r="83">
       <c r="B83" s="0">
-        <v>520470.98888888885</v>
+        <v>520165.9068965518</v>
       </c>
       <c r="C83" s="0">
-        <v>515471.7770833333</v>
+        <v>515164.3116379311</v>
       </c>
       <c r="D83" s="0">
-        <v>510472.5652777777</v>
+        <v>510162.7163793104</v>
       </c>
       <c r="E83" s="0">
         <v>9.962143853357243E-05</v>
       </c>
       <c r="H83" s="0">
-        <v>1273.0688888888833</v>
+        <v>857.7430769230768</v>
       </c>
       <c r="I83" s="0">
-        <v>847.4420833333278</v>
+        <v>428.8715384615384</v>
       </c>
       <c r="J83" s="0">
-        <v>421.8152777777723</v>
+        <v>0</v>
       </c>
       <c r="K83" s="0">
-        <v>0.04715306458123344</v>
+        <v>0.0505634751961274</v>
       </c>
       <c r="N83" s="0">
         <v>-1182315.7222222222</v>
@@ -5153,28 +5153,28 @@
     </row>
     <row r="84">
       <c r="B84" s="0">
-        <v>530469.4125</v>
+        <v>530169.0974137932</v>
       </c>
       <c r="C84" s="0">
-        <v>525470.2006944444</v>
+        <v>525167.5021551725</v>
       </c>
       <c r="D84" s="0">
-        <v>520470.98888888885</v>
+        <v>520165.9068965518</v>
       </c>
       <c r="E84" s="0">
-        <v>0.00023249197934138344</v>
+        <v>0.00018268126007459722</v>
       </c>
       <c r="H84" s="0">
-        <v>2124.3224999999948</v>
+        <v>1715.4861538461537</v>
       </c>
       <c r="I84" s="0">
-        <v>1698.6956944444391</v>
+        <v>1286.6146153846153</v>
       </c>
       <c r="J84" s="0">
-        <v>1273.0688888888835</v>
+        <v>857.7430769230768</v>
       </c>
       <c r="K84" s="0">
-        <v>0.04413912168782915</v>
+        <v>0.04603575127091032</v>
       </c>
       <c r="N84" s="0">
         <v>-1181387.88125</v>
@@ -5215,28 +5215,28 @@
     </row>
     <row r="85">
       <c r="B85" s="0">
-        <v>540467.8361111111</v>
+        <v>540172.2879310346</v>
       </c>
       <c r="C85" s="0">
-        <v>535468.6243055555</v>
+        <v>535170.6926724139</v>
       </c>
       <c r="D85" s="0">
-        <v>530469.4125</v>
+        <v>530169.0974137932</v>
       </c>
       <c r="E85" s="0">
-        <v>8.305982154102482E-05</v>
+        <v>0.00013287054080781102</v>
       </c>
       <c r="H85" s="0">
-        <v>2975.576111111106</v>
+        <v>2573.2292307692305</v>
       </c>
       <c r="I85" s="0">
-        <v>2549.9493055555504</v>
+        <v>2144.357692307692</v>
       </c>
       <c r="J85" s="0">
-        <v>2124.3224999999948</v>
+        <v>1715.4861538461537</v>
       </c>
       <c r="K85" s="0">
-        <v>0.04716062933505791</v>
+        <v>0.04295837912494357</v>
       </c>
       <c r="N85" s="0">
         <v>-1180460.0402777777</v>
@@ -5277,28 +5277,28 @@
     </row>
     <row r="86">
       <c r="B86" s="0">
-        <v>550466.2597222222</v>
+        <v>550175.478448276</v>
       </c>
       <c r="C86" s="0">
-        <v>545467.0479166666</v>
+        <v>545173.8831896553</v>
       </c>
       <c r="D86" s="0">
-        <v>540467.8361111111</v>
+        <v>540172.2879310346</v>
       </c>
       <c r="E86" s="0">
         <v>0.00023249197934138344</v>
       </c>
       <c r="H86" s="0">
-        <v>3826.8297222222172</v>
+        <v>3430.9723076923074</v>
       </c>
       <c r="I86" s="0">
-        <v>3401.2029166666616</v>
+        <v>3002.100769230769</v>
       </c>
       <c r="J86" s="0">
-        <v>2975.576111111106</v>
+        <v>2573.2292307692305</v>
       </c>
       <c r="K86" s="0">
-        <v>0.039374320997944204</v>
+        <v>0.04669206944813974</v>
       </c>
       <c r="N86" s="0">
         <v>-1179532.1993055556</v>
@@ -5339,28 +5339,28 @@
     </row>
     <row r="87">
       <c r="B87" s="0">
-        <v>560464.6833333333</v>
+        <v>560178.6689655173</v>
       </c>
       <c r="C87" s="0">
-        <v>555465.4715277777</v>
+        <v>555177.0737068966</v>
       </c>
       <c r="D87" s="0">
-        <v>550466.2597222222</v>
+        <v>550175.478448276</v>
       </c>
       <c r="E87" s="0">
         <v>0.00018268126007459722</v>
       </c>
       <c r="H87" s="0">
-        <v>4678.0833333333285</v>
+        <v>4288.715384615384</v>
       </c>
       <c r="I87" s="0">
-        <v>4252.456527777773</v>
+        <v>3859.843846153846</v>
       </c>
       <c r="J87" s="0">
-        <v>3826.8297222222172</v>
+        <v>3430.9723076923074</v>
       </c>
       <c r="K87" s="0">
-        <v>0.030356538149181357</v>
+        <v>0.03366783048023545</v>
       </c>
       <c r="N87" s="0">
         <v>-1178604.3583333334</v>
@@ -5401,28 +5401,28 @@
     </row>
     <row r="88">
       <c r="B88" s="0">
-        <v>570463.1069444445</v>
+        <v>570181.8594827587</v>
       </c>
       <c r="C88" s="0">
-        <v>565463.8951388889</v>
+        <v>565180.264224138</v>
       </c>
       <c r="D88" s="0">
-        <v>560464.6833333333</v>
+        <v>560178.6689655173</v>
       </c>
       <c r="E88" s="0">
         <v>0.00023249197934138344</v>
       </c>
       <c r="H88" s="0">
-        <v>5529.33694444444</v>
+        <v>5146.458461538461</v>
       </c>
       <c r="I88" s="0">
-        <v>5103.710138888884</v>
+        <v>4717.586923076922</v>
       </c>
       <c r="J88" s="0">
-        <v>4678.0833333333285</v>
+        <v>4288.715384615384</v>
       </c>
       <c r="K88" s="0">
-        <v>0.02572965483326212</v>
+        <v>0.027128012796227882</v>
       </c>
       <c r="N88" s="0">
         <v>-1177676.5173611112</v>
@@ -5463,28 +5463,28 @@
     </row>
     <row r="89">
       <c r="B89" s="0">
-        <v>580461.5305555556</v>
+        <v>580185.05</v>
       </c>
       <c r="C89" s="0">
-        <v>575462.31875</v>
+        <v>575183.4547413794</v>
       </c>
       <c r="D89" s="0">
-        <v>570463.1069444445</v>
+        <v>570181.8594827587</v>
       </c>
       <c r="E89" s="0">
         <v>8.305982154102482E-05</v>
       </c>
       <c r="H89" s="0">
-        <v>6380.590555555551</v>
+        <v>6004.201538461538</v>
       </c>
       <c r="I89" s="0">
-        <v>5954.963749999995</v>
+        <v>5575.33</v>
       </c>
       <c r="J89" s="0">
-        <v>5529.33694444444</v>
+        <v>5146.458461538461</v>
       </c>
       <c r="K89" s="0">
-        <v>0.03087914581444179</v>
+        <v>0.02832156961423901</v>
       </c>
       <c r="N89" s="0">
         <v>-1176748.6763888889</v>
@@ -5525,28 +5525,28 @@
     </row>
     <row r="90">
       <c r="B90" s="0">
-        <v>590459.9541666667</v>
+        <v>590188.2405172414</v>
       </c>
       <c r="C90" s="0">
-        <v>585460.7423611111</v>
+        <v>585186.6452586207</v>
       </c>
       <c r="D90" s="0">
-        <v>580461.5305555556</v>
+        <v>580185.05</v>
       </c>
       <c r="E90" s="0">
         <v>3.32491022742386E-05</v>
       </c>
       <c r="H90" s="0">
-        <v>7231.844166666662</v>
+        <v>6861.944615384615</v>
       </c>
       <c r="I90" s="0">
-        <v>6806.217361111107</v>
+        <v>6433.073076923076</v>
       </c>
       <c r="J90" s="0">
-        <v>6380.590555555551</v>
+        <v>6004.201538461538</v>
       </c>
       <c r="K90" s="0">
-        <v>0.025472486088710347</v>
+        <v>0.03067683366692558</v>
       </c>
       <c r="N90" s="0">
         <v>-1175820.8354166667</v>
@@ -5587,28 +5587,28 @@
     </row>
     <row r="91">
       <c r="B91" s="0">
-        <v>600458.3777777777</v>
+        <v>600191.4310344828</v>
       </c>
       <c r="C91" s="0">
-        <v>595459.1659722221</v>
+        <v>595189.8357758621</v>
       </c>
       <c r="D91" s="0">
-        <v>590459.9541666666</v>
+        <v>590188.2405172414</v>
       </c>
       <c r="E91" s="0">
         <v>8.305982154102482E-05</v>
       </c>
       <c r="H91" s="0">
-        <v>8083.097777777773</v>
+        <v>7719.687692307692</v>
       </c>
       <c r="I91" s="0">
-        <v>7657.470972222218</v>
+        <v>7290.816153846154</v>
       </c>
       <c r="J91" s="0">
-        <v>7231.844166666662</v>
+        <v>6861.944615384615</v>
       </c>
       <c r="K91" s="0">
-        <v>0.021975824335092185</v>
+        <v>0.0237075948687605</v>
       </c>
       <c r="N91" s="0">
         <v>-1174892.9944444445</v>
@@ -5649,28 +5649,28 @@
     </row>
     <row r="92">
       <c r="B92" s="0">
-        <v>610456.8013888889</v>
+        <v>610194.6215517243</v>
       </c>
       <c r="C92" s="0">
-        <v>605457.5895833332</v>
+        <v>605193.0262931036</v>
       </c>
       <c r="D92" s="0">
-        <v>600458.3777777777</v>
+        <v>600191.4310344829</v>
       </c>
       <c r="E92" s="0">
         <v>0.00018268126007459722</v>
       </c>
       <c r="H92" s="0">
-        <v>8934.351388888885</v>
+        <v>8577.430769230768</v>
       </c>
       <c r="I92" s="0">
-        <v>8508.724583333329</v>
+        <v>8148.5592307692295</v>
       </c>
       <c r="J92" s="0">
-        <v>8083.097777777773</v>
+        <v>7719.687692307692</v>
       </c>
       <c r="K92" s="0">
-        <v>0.011933330077658549</v>
+        <v>0.015158452846786654</v>
       </c>
       <c r="N92" s="0">
         <v>-1173965.1534722222</v>
@@ -5711,28 +5711,28 @@
     </row>
     <row r="93">
       <c r="B93" s="0">
-        <v>620455.225</v>
+        <v>620197.8120689656</v>
       </c>
       <c r="C93" s="0">
-        <v>615456.0131944444</v>
+        <v>615196.216810345</v>
       </c>
       <c r="D93" s="0">
-        <v>610456.8013888889</v>
+        <v>610194.6215517243</v>
       </c>
       <c r="E93" s="0">
         <v>0.00018268126007459722</v>
       </c>
       <c r="H93" s="0">
-        <v>9785.604999999996</v>
+        <v>9435.173846153844</v>
       </c>
       <c r="I93" s="0">
-        <v>9359.97819444444</v>
+        <v>9006.302307692307</v>
       </c>
       <c r="J93" s="0">
-        <v>8934.351388888885</v>
+        <v>8577.430769230768</v>
       </c>
       <c r="K93" s="0">
-        <v>0.007877146089899593</v>
+        <v>0.009439813745315776</v>
       </c>
       <c r="N93" s="0">
         <v>-1173037.3125</v>
@@ -5773,28 +5773,28 @@
     </row>
     <row r="94">
       <c r="B94" s="0">
-        <v>630453.6486111111</v>
+        <v>630201.002586207</v>
       </c>
       <c r="C94" s="0">
-        <v>625454.4368055555</v>
+        <v>625199.4073275863</v>
       </c>
       <c r="D94" s="0">
-        <v>620455.225</v>
+        <v>620197.8120689656</v>
       </c>
       <c r="E94" s="0">
         <v>0.00013287054080781102</v>
       </c>
       <c r="H94" s="0">
-        <v>10636.858611111107</v>
+        <v>10292.916923076922</v>
       </c>
       <c r="I94" s="0">
-        <v>10211.231805555552</v>
+        <v>9864.045384615383</v>
       </c>
       <c r="J94" s="0">
-        <v>9785.604999999996</v>
+        <v>9435.173846153844</v>
       </c>
       <c r="K94" s="0">
-        <v>0.00568303992702775</v>
+        <v>0.006148611164905535</v>
       </c>
       <c r="N94" s="0">
         <v>-1172109.4715277778</v>
@@ -5835,28 +5835,28 @@
     </row>
     <row r="95">
       <c r="B95" s="0">
-        <v>640452.0722222222</v>
+        <v>640204.1931034484</v>
       </c>
       <c r="C95" s="0">
-        <v>635452.8604166666</v>
+        <v>635202.5978448277</v>
       </c>
       <c r="D95" s="0">
-        <v>630453.6486111111</v>
+        <v>630201.002586207</v>
       </c>
       <c r="E95" s="0">
         <v>0.0006309777334756731</v>
       </c>
       <c r="H95" s="0">
-        <v>11488.112222222218</v>
+        <v>11150.66</v>
       </c>
       <c r="I95" s="0">
-        <v>11062.485416666663</v>
+        <v>10721.788461538461</v>
       </c>
       <c r="J95" s="0">
-        <v>10636.858611111107</v>
+        <v>10292.916923076922</v>
       </c>
       <c r="K95" s="0">
-        <v>0.0035713636073253156</v>
+        <v>0.004153244724407206</v>
       </c>
       <c r="N95" s="0">
         <v>-1171181.6305555555</v>
@@ -5897,28 +5897,28 @@
     </row>
     <row r="96">
       <c r="B96" s="0">
-        <v>650450.4958333333</v>
+        <v>650207.3836206897</v>
       </c>
       <c r="C96" s="0">
-        <v>645451.2840277777</v>
+        <v>645205.788362069</v>
       </c>
       <c r="D96" s="0">
-        <v>640452.0722222222</v>
+        <v>640204.1931034484</v>
       </c>
       <c r="E96" s="0">
-        <v>0.0004815455756753146</v>
+        <v>0.0004317348564085284</v>
       </c>
       <c r="H96" s="0">
-        <v>12339.36583333333</v>
+        <v>12008.403076923078</v>
       </c>
       <c r="I96" s="0">
-        <v>11913.739027777774</v>
+        <v>11579.531538461539</v>
       </c>
       <c r="J96" s="0">
-        <v>11488.112222222218</v>
+        <v>11150.66</v>
       </c>
       <c r="K96" s="0">
-        <v>0.002441354903981188</v>
+        <v>0.0026739727516117144</v>
       </c>
       <c r="N96" s="0">
         <v>-1170253.7895833333</v>
@@ -5959,28 +5959,28 @@
     </row>
     <row r="97">
       <c r="B97" s="0">
-        <v>660448.9194444445</v>
+        <v>660210.5741379311</v>
       </c>
       <c r="C97" s="0">
-        <v>655449.7076388889</v>
+        <v>655208.9788793104</v>
       </c>
       <c r="D97" s="0">
-        <v>650450.4958333333</v>
+        <v>650207.3836206897</v>
       </c>
       <c r="E97" s="0">
-        <v>0.0006807884527424593</v>
+        <v>0.0007305991720092455</v>
       </c>
       <c r="H97" s="0">
-        <v>13190.61944444444</v>
+        <v>12866.146153846152</v>
       </c>
       <c r="I97" s="0">
-        <v>12764.992638888885</v>
+        <v>12437.274615384615</v>
       </c>
       <c r="J97" s="0">
-        <v>12339.36583333333</v>
+        <v>12008.403076923076</v>
       </c>
       <c r="K97" s="0">
-        <v>0.0023747725749313177</v>
+        <v>0.002474519881754033</v>
       </c>
       <c r="N97" s="0">
         <v>-1169325.9486111111</v>
@@ -6021,28 +6021,28 @@
     </row>
     <row r="98">
       <c r="B98" s="0">
-        <v>670447.3430555556</v>
+        <v>670213.7646551725</v>
       </c>
       <c r="C98" s="0">
-        <v>665448.13125</v>
+        <v>665212.1693965518</v>
       </c>
       <c r="D98" s="0">
-        <v>660448.9194444445</v>
+        <v>660210.5741379311</v>
       </c>
       <c r="E98" s="0">
         <v>0.0006309777334756731</v>
       </c>
       <c r="H98" s="0">
-        <v>14041.873055555552</v>
+        <v>13723.88923076923</v>
       </c>
       <c r="I98" s="0">
-        <v>13616.246249999997</v>
+        <v>13295.01769230769</v>
       </c>
       <c r="J98" s="0">
-        <v>13190.61944444444</v>
+        <v>12866.146153846152</v>
       </c>
       <c r="K98" s="0">
-        <v>0.002075530654463171</v>
+        <v>0.0025405566753966347</v>
       </c>
       <c r="N98" s="0">
         <v>-1168398.107638889</v>
@@ -6083,28 +6083,28 @@
     </row>
     <row r="99">
       <c r="B99" s="0">
-        <v>680445.7666666667</v>
+        <v>680216.9551724138</v>
       </c>
       <c r="C99" s="0">
-        <v>675446.5548611111</v>
+        <v>675215.3599137932</v>
       </c>
       <c r="D99" s="0">
-        <v>670447.3430555556</v>
+        <v>670213.7646551725</v>
       </c>
       <c r="E99" s="0">
         <v>0.0003321134178749559</v>
       </c>
       <c r="H99" s="0">
-        <v>14893.126666666663</v>
+        <v>14581.632307692307</v>
       </c>
       <c r="I99" s="0">
-        <v>14467.499861111108</v>
+        <v>14152.760769230768</v>
       </c>
       <c r="J99" s="0">
-        <v>14041.873055555552</v>
+        <v>13723.88923076923</v>
       </c>
       <c r="K99" s="0">
-        <v>0.001892807332137877</v>
+        <v>0.0014445108587368004</v>
       </c>
       <c r="N99" s="0">
         <v>-1167470.2666666666</v>
@@ -6145,28 +6145,28 @@
     </row>
     <row r="100">
       <c r="B100" s="0">
-        <v>690444.1902777778</v>
+        <v>690220.1456896552</v>
       </c>
       <c r="C100" s="0">
-        <v>685444.9784722222</v>
+        <v>685218.5504310345</v>
       </c>
       <c r="D100" s="0">
-        <v>680445.7666666667</v>
+        <v>680216.9551724138</v>
       </c>
       <c r="E100" s="0">
-        <v>0.000880031329809604</v>
+        <v>0.0008302206105428178</v>
       </c>
       <c r="H100" s="0">
-        <v>15744.38027777776</v>
+        <v>15439.375384615385</v>
       </c>
       <c r="I100" s="0">
-        <v>15318.753472222204</v>
+        <v>15010.503846153846</v>
       </c>
       <c r="J100" s="0">
-        <v>14893.126666666649</v>
+        <v>14581.632307692307</v>
       </c>
       <c r="K100" s="0">
-        <v>0.0009464036660689377</v>
+        <v>0.0015939430165371592</v>
       </c>
       <c r="N100" s="0">
         <v>-1166542.4256944444</v>
@@ -6207,28 +6207,28 @@
     </row>
     <row r="101">
       <c r="B101" s="0">
-        <v>700442.6138888889</v>
+        <v>700223.3362068967</v>
       </c>
       <c r="C101" s="0">
-        <v>695443.4020833332</v>
+        <v>695221.740948276</v>
       </c>
       <c r="D101" s="0">
-        <v>690444.1902777777</v>
+        <v>690220.1456896553</v>
       </c>
       <c r="E101" s="0">
-        <v>0.0002823026986081697</v>
+        <v>0.0003321134178749559</v>
       </c>
       <c r="H101" s="0">
-        <v>16595.63388888887</v>
+        <v>16297.118461538459</v>
       </c>
       <c r="I101" s="0">
-        <v>16170.007083333316</v>
+        <v>15868.246923076922</v>
       </c>
       <c r="J101" s="0">
-        <v>15744.38027777776</v>
+        <v>15439.375384615383</v>
       </c>
       <c r="K101" s="0">
-        <v>0.0010958358238692964</v>
+        <v>0.0009962143853357239</v>
       </c>
       <c r="N101" s="0">
         <v>-1165614.5847222223</v>
@@ -6269,28 +6269,28 @@
     </row>
     <row r="102">
       <c r="B102" s="0">
-        <v>710441.0375</v>
+        <v>710226.5267241381</v>
       </c>
       <c r="C102" s="0">
-        <v>705441.8256944444</v>
+        <v>705224.9314655174</v>
       </c>
       <c r="D102" s="0">
-        <v>700442.6138888889</v>
+        <v>700223.3362068967</v>
       </c>
       <c r="E102" s="0">
         <v>0.0005313562949421008</v>
       </c>
       <c r="H102" s="0">
-        <v>17446.887499999983</v>
+        <v>17154.861538461537</v>
       </c>
       <c r="I102" s="0">
-        <v>17021.260694444427</v>
+        <v>16725.989999999998</v>
       </c>
       <c r="J102" s="0">
-        <v>16595.63388888887</v>
+        <v>16297.118461538459</v>
       </c>
       <c r="K102" s="0">
-        <v>0.0006475393504682207</v>
+        <v>0.0007969715082685792</v>
       </c>
       <c r="N102" s="0">
         <v>-1164686.74375</v>
@@ -6331,28 +6331,28 @@
     </row>
     <row r="103">
       <c r="B103" s="0">
-        <v>720439.4611111111</v>
+        <v>720229.7172413794</v>
       </c>
       <c r="C103" s="0">
-        <v>715440.2493055555</v>
+        <v>715228.1219827587</v>
       </c>
       <c r="D103" s="0">
-        <v>710441.0375</v>
+        <v>710226.5267241381</v>
       </c>
       <c r="E103" s="0">
         <v>0.0003321134178749559</v>
       </c>
       <c r="H103" s="0">
-        <v>18298.141111111094</v>
+        <v>18012.604615384615</v>
       </c>
       <c r="I103" s="0">
-        <v>17872.514305555538</v>
+        <v>17583.733076923076</v>
       </c>
       <c r="J103" s="0">
-        <v>17446.887499999983</v>
+        <v>17154.861538461537</v>
       </c>
       <c r="K103" s="0">
-        <v>0.0005977286312014345</v>
+        <v>0.0006475393504682207</v>
       </c>
       <c r="N103" s="0">
         <v>-1163758.9027777778</v>
@@ -6379,39 +6379,39 @@
         <v>0.006504933249363181</v>
       </c>
       <c r="Z103" s="0">
-        <v>40664.37499999962</v>
+        <v>0</v>
       </c>
       <c r="AA103" s="0">
-        <v>7155.378124999625</v>
+        <v>-13176.809375000375</v>
       </c>
       <c r="AB103" s="0">
-        <v>-26353.618750000373</v>
+        <v>-26353.61875000075</v>
       </c>
       <c r="AC103" s="0">
-        <v>0.12968613706252186</v>
+        <v>0.04227535069955335</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" s="0">
-        <v>730437.8847222222</v>
+        <v>730232.9077586208</v>
       </c>
       <c r="C104" s="0">
-        <v>725438.6729166666</v>
+        <v>725231.3125000001</v>
       </c>
       <c r="D104" s="0">
-        <v>720439.4611111111</v>
+        <v>720229.7172413794</v>
       </c>
       <c r="E104" s="0">
         <v>0.0003321134178749559</v>
       </c>
       <c r="H104" s="0">
-        <v>19149.394722222205</v>
+        <v>18870.347692307692</v>
       </c>
       <c r="I104" s="0">
-        <v>18723.76791666665</v>
+        <v>18441.476153846153</v>
       </c>
       <c r="J104" s="0">
-        <v>18298.141111111094</v>
+        <v>18012.604615384615</v>
       </c>
       <c r="K104" s="0">
         <v>0.0005479179119346483</v>
@@ -6441,39 +6441,39 @@
         <v>0.006039908183818557</v>
       </c>
       <c r="Z104" s="0">
-        <v>107682.36874999906</v>
+        <v>67942.1840909091</v>
       </c>
       <c r="AA104" s="0">
-        <v>74173.37187499907</v>
+        <v>33971.09204545455</v>
       </c>
       <c r="AB104" s="0">
-        <v>40664.37499999907</v>
+        <v>0</v>
       </c>
       <c r="AC104" s="0">
-        <v>0.05247933231347929</v>
+        <v>0.11267773170167243</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" s="0">
-        <v>740436.3083333333</v>
+        <v>740236.0982758622</v>
       </c>
       <c r="C105" s="0">
-        <v>735437.0965277777</v>
+        <v>735234.5030172415</v>
       </c>
       <c r="D105" s="0">
-        <v>730437.8847222222</v>
+        <v>730232.9077586208</v>
       </c>
       <c r="E105" s="0">
         <v>0.0003321134178749559</v>
       </c>
       <c r="H105" s="0">
-        <v>20000.648333333316</v>
+        <v>19728.090769230766</v>
       </c>
       <c r="I105" s="0">
-        <v>19575.02152777776</v>
+        <v>19299.219230769228</v>
       </c>
       <c r="J105" s="0">
-        <v>19149.394722222205</v>
+        <v>18870.34769230769</v>
       </c>
       <c r="K105" s="0">
         <v>0.00034867503486750353</v>
@@ -6503,42 +6503,42 @@
         <v>0.005075095346355891</v>
       </c>
       <c r="Z105" s="0">
-        <v>174700.36249999944</v>
+        <v>135884.3681818182</v>
       </c>
       <c r="AA105" s="0">
-        <v>141191.36562499945</v>
+        <v>101913.27613636365</v>
       </c>
       <c r="AB105" s="0">
-        <v>107682.36874999944</v>
+        <v>67942.1840909091</v>
       </c>
       <c r="AC105" s="0">
-        <v>0.04190032402741629</v>
+        <v>0.04667638107683553</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" s="0">
-        <v>750434.7319444445</v>
+        <v>750239.2887931035</v>
       </c>
       <c r="C106" s="0">
-        <v>745435.5201388889</v>
+        <v>745237.6935344829</v>
       </c>
       <c r="D106" s="0">
-        <v>740436.3083333333</v>
+        <v>740236.0982758622</v>
       </c>
       <c r="E106" s="0">
         <v>0.0006309777334756731</v>
       </c>
       <c r="H106" s="0">
-        <v>20851.901944444427</v>
+        <v>20585.833846153844</v>
       </c>
       <c r="I106" s="0">
-        <v>20426.275138888872</v>
+        <v>20156.962307692305</v>
       </c>
       <c r="J106" s="0">
-        <v>20000.648333333316</v>
+        <v>19728.090769230766</v>
       </c>
       <c r="K106" s="0">
-        <v>0.00034867503486750353</v>
+        <v>0.0002490535963339311</v>
       </c>
       <c r="N106" s="0">
         <v>-1160975.379861111</v>
@@ -6565,42 +6565,42 @@
         <v>0.0047587035743113385</v>
       </c>
       <c r="Z106" s="0">
-        <v>241718.3562499998</v>
+        <v>203826.5522727273</v>
       </c>
       <c r="AA106" s="0">
-        <v>208209.35937499983</v>
+        <v>169855.46022727274</v>
       </c>
       <c r="AB106" s="0">
-        <v>174700.3624999998</v>
+        <v>135884.3681818182</v>
       </c>
       <c r="AC106" s="0">
-        <v>0.03922425644330664</v>
+        <v>0.04050289748476193</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" s="0">
-        <v>760433.1555555556</v>
+        <v>760242.4793103449</v>
       </c>
       <c r="C107" s="0">
-        <v>755433.94375</v>
+        <v>755240.8840517242</v>
       </c>
       <c r="D107" s="0">
-        <v>750434.7319444445</v>
+        <v>750239.2887931035</v>
       </c>
       <c r="E107" s="0">
         <v>0.0002823026986081697</v>
       </c>
       <c r="H107" s="0">
-        <v>21703.15555555554</v>
+        <v>21443.576923076922</v>
       </c>
       <c r="I107" s="0">
-        <v>21277.528749999983</v>
+        <v>21014.705384615383</v>
       </c>
       <c r="J107" s="0">
-        <v>20851.901944444427</v>
+        <v>20585.833846153844</v>
       </c>
       <c r="K107" s="0">
-        <v>0.000747160789001793</v>
+        <v>0.0007969715082685792</v>
       </c>
       <c r="N107" s="0">
         <v>-1160047.538888889</v>
@@ -6627,39 +6627,39 @@
         <v>0.004143741285495057</v>
       </c>
       <c r="Z107" s="0">
-        <v>308736.3499999993</v>
+        <v>271768.7363636364</v>
       </c>
       <c r="AA107" s="0">
-        <v>275227.35312499927</v>
+        <v>237797.64431818185</v>
       </c>
       <c r="AB107" s="0">
-        <v>241718.35624999925</v>
+        <v>203826.5522727273</v>
       </c>
       <c r="AC107" s="0">
-        <v>0.03173377669713687</v>
+        <v>0.036483532795179165</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" s="0">
-        <v>770431.5791666667</v>
+        <v>770245.6698275863</v>
       </c>
       <c r="C108" s="0">
-        <v>765432.3673611111</v>
+        <v>765244.0745689656</v>
       </c>
       <c r="D108" s="0">
-        <v>760433.1555555556</v>
+        <v>760242.4793103449</v>
       </c>
       <c r="E108" s="0">
         <v>0.00018268126007459722</v>
       </c>
       <c r="H108" s="0">
-        <v>22554.40916666665</v>
+        <v>22301.32</v>
       </c>
       <c r="I108" s="0">
-        <v>22128.782361111094</v>
+        <v>21872.44846153846</v>
       </c>
       <c r="J108" s="0">
-        <v>21703.15555555554</v>
+        <v>21443.576923076922</v>
       </c>
       <c r="K108" s="0">
         <v>0.000747160789001793</v>
@@ -6689,42 +6689,42 @@
         <v>0.004476190882912635</v>
       </c>
       <c r="Z108" s="0">
-        <v>375754.34374999965</v>
+        <v>339710.92045454547</v>
       </c>
       <c r="AA108" s="0">
-        <v>342245.34687499964</v>
+        <v>305739.82840909093</v>
       </c>
       <c r="AB108" s="0">
-        <v>308736.3499999996</v>
+        <v>271768.7363636364</v>
       </c>
       <c r="AC108" s="0">
-        <v>0.02312854689023329</v>
+        <v>0.029126133582607936</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" s="0">
-        <v>780430.0027777778</v>
+        <v>780248.8603448276</v>
       </c>
       <c r="C109" s="0">
-        <v>775430.7909722222</v>
+        <v>775247.265086207</v>
       </c>
       <c r="D109" s="0">
-        <v>770431.5791666667</v>
+        <v>770245.6698275863</v>
       </c>
       <c r="E109" s="0">
         <v>0.00011630892381526341</v>
       </c>
       <c r="H109" s="0">
-        <v>23405.66277777776</v>
+        <v>23159.063076923077</v>
       </c>
       <c r="I109" s="0">
-        <v>22980.035972222206</v>
+        <v>22730.19153846154</v>
       </c>
       <c r="J109" s="0">
-        <v>22554.40916666665</v>
+        <v>22301.32</v>
       </c>
       <c r="K109" s="0">
-        <v>0.00034867503486750353</v>
+        <v>0.000448296473401076</v>
       </c>
       <c r="N109" s="0">
         <v>-1158191.8569444444</v>
@@ -6751,42 +6751,42 @@
         <v>0.00381108169528694</v>
       </c>
       <c r="Z109" s="0">
-        <v>442772.3374999991</v>
+        <v>407653.10454545455</v>
       </c>
       <c r="AA109" s="0">
-        <v>409263.3406249991</v>
+        <v>373682.0125</v>
       </c>
       <c r="AB109" s="0">
-        <v>375754.34374999907</v>
+        <v>339710.92045454547</v>
       </c>
       <c r="AC109" s="0">
-        <v>0.022206392360683055</v>
+        <v>0.02127251743094693</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" s="0">
-        <v>790428.4263888889</v>
+        <v>790252.0508620691</v>
       </c>
       <c r="C110" s="0">
-        <v>785429.2145833332</v>
+        <v>785250.4556034484</v>
       </c>
       <c r="D110" s="0">
-        <v>780430.0027777777</v>
+        <v>780248.8603448278</v>
       </c>
       <c r="E110" s="0">
         <v>0.00018268126007459722</v>
       </c>
       <c r="H110" s="0">
-        <v>24256.916388888872</v>
+        <v>24016.80615384615</v>
       </c>
       <c r="I110" s="0">
-        <v>23831.289583333317</v>
+        <v>23587.934615384613</v>
       </c>
       <c r="J110" s="0">
-        <v>23405.66277777776</v>
+        <v>23159.063076923074</v>
       </c>
       <c r="K110" s="0">
-        <v>0.0004981071926678622</v>
+        <v>0.00039848575413428976</v>
       </c>
       <c r="N110" s="0">
         <v>-1157264.0159722222</v>
@@ -6813,42 +6813,42 @@
         <v>0.004126591752381598</v>
       </c>
       <c r="Z110" s="0">
-        <v>509790.33124999946</v>
+        <v>475595.2886363637</v>
       </c>
       <c r="AA110" s="0">
-        <v>476281.33437499945</v>
+        <v>441624.19659090915</v>
       </c>
       <c r="AB110" s="0">
-        <v>442772.33749999944</v>
+        <v>407653.1045454546</v>
       </c>
       <c r="AC110" s="0">
-        <v>0.018367353763598947</v>
+        <v>0.02046217689672045</v>
       </c>
     </row>
     <row r="111">
       <c r="B111" s="0">
-        <v>800426.8500000001</v>
+        <v>800255.2413793105</v>
       </c>
       <c r="C111" s="0">
-        <v>795427.6381944445</v>
+        <v>795253.6461206898</v>
       </c>
       <c r="D111" s="0">
-        <v>790428.426388889</v>
+        <v>790252.0508620691</v>
       </c>
       <c r="E111" s="0">
         <v>3.32491022742386E-05</v>
       </c>
       <c r="H111" s="0">
-        <v>25108.169999999984</v>
+        <v>24874.54923076923</v>
       </c>
       <c r="I111" s="0">
-        <v>24682.543194444428</v>
+        <v>24445.67769230769</v>
       </c>
       <c r="J111" s="0">
-        <v>24256.916388888872</v>
+        <v>24016.80615384615</v>
       </c>
       <c r="K111" s="0">
-        <v>0.00039848575413428976</v>
+        <v>0.0004981071926678622</v>
       </c>
       <c r="N111" s="0">
         <v>-1156336.175</v>
@@ -6875,42 +6875,42 @@
         <v>0.0031615679667395583</v>
       </c>
       <c r="Z111" s="0">
-        <v>576808.3249999998</v>
+        <v>543537.4727272728</v>
       </c>
       <c r="AA111" s="0">
-        <v>543299.3281249998</v>
+        <v>509566.38068181823</v>
       </c>
       <c r="AB111" s="0">
-        <v>509790.3312499998</v>
+        <v>475595.2886363637</v>
       </c>
       <c r="AC111" s="0">
-        <v>0.018333432302239463</v>
+        <v>0.01803339183593397</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" s="0">
-        <v>810425.2736111111</v>
+        <v>810258.4318965519</v>
       </c>
       <c r="C112" s="0">
-        <v>805426.0618055555</v>
+        <v>805256.8366379312</v>
       </c>
       <c r="D112" s="0">
-        <v>800426.85</v>
+        <v>800255.2413793105</v>
       </c>
       <c r="E112" s="0">
         <v>0.00018268126007459722</v>
       </c>
       <c r="H112" s="0">
-        <v>25959.423611111095</v>
+        <v>25732.292307692307</v>
       </c>
       <c r="I112" s="0">
-        <v>25533.79680555554</v>
+        <v>25303.42076923077</v>
       </c>
       <c r="J112" s="0">
-        <v>25108.169999999984</v>
+        <v>24874.54923076923</v>
       </c>
       <c r="K112" s="0">
-        <v>0.0002988643156007173</v>
+        <v>0.0002490535963339311</v>
       </c>
       <c r="N112" s="0">
         <v>-1155408.3340277777</v>
@@ -6937,42 +6937,42 @@
         <v>0.003527181905004093</v>
       </c>
       <c r="Z112" s="0">
-        <v>643826.3187499993</v>
+        <v>611479.6568181819</v>
       </c>
       <c r="AA112" s="0">
-        <v>610317.3218749992</v>
+        <v>577508.5647727273</v>
       </c>
       <c r="AB112" s="0">
-        <v>576808.3249999993</v>
+        <v>543537.4727272728</v>
       </c>
       <c r="AC112" s="0">
-        <v>0.01807029557707462</v>
+        <v>0.018701483621803766</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" s="0">
-        <v>820423.6972222223</v>
+        <v>820261.6224137932</v>
       </c>
       <c r="C113" s="0">
-        <v>815424.4854166667</v>
+        <v>815260.0271551725</v>
       </c>
       <c r="D113" s="0">
-        <v>810425.2736111112</v>
+        <v>810258.4318965519</v>
       </c>
       <c r="E113" s="0">
         <v>8.305982154102482E-05</v>
       </c>
       <c r="H113" s="0">
-        <v>26810.677222222206</v>
+        <v>26590.03538461538</v>
       </c>
       <c r="I113" s="0">
-        <v>26385.05041666665</v>
+        <v>26161.163846153842</v>
       </c>
       <c r="J113" s="0">
-        <v>25959.423611111095</v>
+        <v>25732.292307692303</v>
       </c>
       <c r="K113" s="0">
-        <v>0.00019924287706714485</v>
+        <v>0.0002988643156007173</v>
       </c>
       <c r="N113" s="0">
         <v>-1154480.4930555555</v>
@@ -6999,42 +6999,42 @@
         <v>0.003160810846227024</v>
       </c>
       <c r="Z113" s="0">
-        <v>710844.3124999997</v>
+        <v>679421.8409090909</v>
       </c>
       <c r="AA113" s="0">
-        <v>677335.3156249996</v>
+        <v>645450.7488636364</v>
       </c>
       <c r="AB113" s="0">
-        <v>643826.3187499996</v>
+        <v>611479.6568181819</v>
       </c>
       <c r="AC113" s="0">
-        <v>0.018835319683599944</v>
+        <v>0.01930030364228271</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" s="0">
-        <v>830422.1208333333</v>
+        <v>830264.8129310346</v>
       </c>
       <c r="C114" s="0">
-        <v>825422.9090277777</v>
+        <v>825263.2176724139</v>
       </c>
       <c r="D114" s="0">
-        <v>820423.6972222222</v>
+        <v>820261.6224137932</v>
       </c>
       <c r="E114" s="0">
-        <v>0.00036536252014919454</v>
+        <v>0.0003321134178749559</v>
       </c>
       <c r="H114" s="0">
-        <v>27661.930833333317</v>
+        <v>27447.77846153846</v>
       </c>
       <c r="I114" s="0">
-        <v>27236.30402777776</v>
+        <v>27018.90692307692</v>
       </c>
       <c r="J114" s="0">
-        <v>26810.677222222206</v>
+        <v>26590.03538461538</v>
       </c>
       <c r="K114" s="0">
-        <v>0.0002988643156007173</v>
+        <v>0.00019924287706714485</v>
       </c>
       <c r="N114" s="0">
         <v>-1153552.6520833333</v>
@@ -7061,42 +7061,42 @@
         <v>0.003260179911256417</v>
       </c>
       <c r="Z114" s="0">
-        <v>777862.3062499991</v>
+        <v>747364.025</v>
       </c>
       <c r="AA114" s="0">
-        <v>744353.309374999</v>
+        <v>713392.9329545455</v>
       </c>
       <c r="AB114" s="0">
-        <v>710844.3124999991</v>
+        <v>679421.8409090909</v>
       </c>
       <c r="AC114" s="0">
-        <v>0.016206200993394676</v>
+        <v>0.016805777497460258</v>
       </c>
     </row>
     <row r="115">
       <c r="B115" s="0">
-        <v>840420.5444444444</v>
+        <v>840268.003448276</v>
       </c>
       <c r="C115" s="0">
-        <v>835421.3326388887</v>
+        <v>835266.4081896553</v>
       </c>
       <c r="D115" s="0">
-        <v>830422.1208333332</v>
+        <v>830264.8129310346</v>
       </c>
       <c r="E115" s="0">
-        <v>0.00023249197934138344</v>
+        <v>0.00026574108161562203</v>
       </c>
       <c r="H115" s="0">
-        <v>28513.18444444443</v>
+        <v>28305.521538461537</v>
       </c>
       <c r="I115" s="0">
-        <v>28087.557638888873</v>
+        <v>27876.649999999998</v>
       </c>
       <c r="J115" s="0">
-        <v>27661.930833333317</v>
+        <v>27447.77846153846</v>
       </c>
       <c r="K115" s="0">
-        <v>0.00034867503486750353</v>
+        <v>0.0004981071926678622</v>
       </c>
       <c r="N115" s="0">
         <v>-1152624.8111111112</v>
@@ -7123,39 +7123,39 @@
         <v>0.003177288657181125</v>
       </c>
       <c r="Z115" s="0">
-        <v>844880.2999999995</v>
+        <v>815306.2090909091</v>
       </c>
       <c r="AA115" s="0">
-        <v>811371.3031249994</v>
+        <v>781335.1170454546</v>
       </c>
       <c r="AB115" s="0">
-        <v>777862.3062499994</v>
+        <v>747364.025</v>
       </c>
       <c r="AC115" s="0">
-        <v>0.014460389393146212</v>
+        <v>0.015475097711302947</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" s="0">
-        <v>850418.9680555556</v>
+        <v>850271.1939655173</v>
       </c>
       <c r="C116" s="0">
-        <v>845419.75625</v>
+        <v>845269.5987068966</v>
       </c>
       <c r="D116" s="0">
-        <v>840420.5444444445</v>
+        <v>840268.003448276</v>
       </c>
       <c r="E116" s="0">
         <v>0.0002823026986081697</v>
       </c>
       <c r="H116" s="0">
-        <v>29364.43805555554</v>
+        <v>29163.264615384614</v>
       </c>
       <c r="I116" s="0">
-        <v>28938.811249999984</v>
+        <v>28734.393076923076</v>
       </c>
       <c r="J116" s="0">
-        <v>28513.18444444443</v>
+        <v>28305.521538461537</v>
       </c>
       <c r="K116" s="0">
         <v>9.962143853357243E-05</v>
@@ -7185,39 +7185,39 @@
         <v>0.0033100750734875433</v>
       </c>
       <c r="Z116" s="0">
-        <v>911898.2937499989</v>
+        <v>883248.3931818183</v>
       </c>
       <c r="AA116" s="0">
-        <v>878389.2968749988</v>
+        <v>849277.3011363638</v>
       </c>
       <c r="AB116" s="0">
-        <v>844880.2999999989</v>
+        <v>815306.2090909092</v>
       </c>
       <c r="AC116" s="0">
-        <v>0.0142599283031236</v>
+        <v>0.014975814367930317</v>
       </c>
     </row>
     <row r="117">
       <c r="B117" s="0">
-        <v>860417.3916666666</v>
+        <v>860274.3844827587</v>
       </c>
       <c r="C117" s="0">
-        <v>855418.179861111</v>
+        <v>855272.789224138</v>
       </c>
       <c r="D117" s="0">
-        <v>850418.9680555555</v>
+        <v>850271.1939655173</v>
       </c>
       <c r="E117" s="0">
         <v>0.0006807884527424593</v>
       </c>
       <c r="H117" s="0">
-        <v>30215.69166666665</v>
+        <v>30021.007692307692</v>
       </c>
       <c r="I117" s="0">
-        <v>29790.064861111096</v>
+        <v>29592.136153846153</v>
       </c>
       <c r="J117" s="0">
-        <v>29364.43805555554</v>
+        <v>29163.264615384614</v>
       </c>
       <c r="K117" s="0">
         <v>9.962143853357243E-05</v>
@@ -7247,39 +7247,39 @@
         <v>0.0018629601767629145</v>
       </c>
       <c r="Z117" s="0">
-        <v>978916.2874999993</v>
+        <v>951190.5772727274</v>
       </c>
       <c r="AA117" s="0">
-        <v>945407.2906249992</v>
+        <v>917219.4852272728</v>
       </c>
       <c r="AB117" s="0">
-        <v>911898.2937499993</v>
+        <v>883248.3931818183</v>
       </c>
       <c r="AC117" s="0">
-        <v>0.012064391705265137</v>
+        <v>0.013345513464122744</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" s="0">
-        <v>870415.8152777778</v>
+        <v>870277.5750000001</v>
       </c>
       <c r="C118" s="0">
-        <v>865416.6034722222</v>
+        <v>865275.9797413794</v>
       </c>
       <c r="D118" s="0">
-        <v>860417.3916666667</v>
+        <v>860274.3844827587</v>
       </c>
       <c r="E118" s="0">
-        <v>0.0007638482742834841</v>
+        <v>0.0007140375550166979</v>
       </c>
       <c r="H118" s="0">
-        <v>31066.945277777762</v>
+        <v>30878.750769230766</v>
       </c>
       <c r="I118" s="0">
-        <v>30641.318472222207</v>
+        <v>30449.879230769227</v>
       </c>
       <c r="J118" s="0">
-        <v>30215.69166666665</v>
+        <v>30021.00769230769</v>
       </c>
       <c r="K118" s="0">
         <v>9.962143853357243E-05</v>
@@ -7309,39 +7309,39 @@
         <v>0.0016455592279544314</v>
       </c>
       <c r="Z118" s="0">
-        <v>1045934.2812499997</v>
+        <v>1019132.7613636365</v>
       </c>
       <c r="AA118" s="0">
-        <v>1012425.2843749996</v>
+        <v>985161.6693181819</v>
       </c>
       <c r="AB118" s="0">
-        <v>978916.2874999996</v>
+        <v>951190.5772727274</v>
       </c>
       <c r="AC118" s="0">
-        <v>0.011813740698793582</v>
+        <v>0.011814539563093867</v>
       </c>
     </row>
     <row r="119">
       <c r="B119" s="0">
-        <v>880414.2388888889</v>
+        <v>880280.7655172416</v>
       </c>
       <c r="C119" s="0">
-        <v>875415.0270833332</v>
+        <v>875279.1702586209</v>
       </c>
       <c r="D119" s="0">
-        <v>870415.8152777777</v>
+        <v>870277.5750000002</v>
       </c>
       <c r="E119" s="0">
-        <v>0.0006309777334756731</v>
+        <v>0.0006807884527424593</v>
       </c>
       <c r="H119" s="0">
-        <v>31918.198888888874</v>
+        <v>31736.493846153844</v>
       </c>
       <c r="I119" s="0">
-        <v>31492.572083333318</v>
+        <v>31307.622307692305</v>
       </c>
       <c r="J119" s="0">
-        <v>31066.945277777762</v>
+        <v>30878.750769230766</v>
       </c>
       <c r="K119" s="0">
         <v>9.962143853357243E-05</v>
@@ -7371,42 +7371,42 @@
         <v>0.0013136146960081555</v>
       </c>
       <c r="Z119" s="0">
-        <v>1112952.274999999</v>
+        <v>1087074.9454545456</v>
       </c>
       <c r="AA119" s="0">
-        <v>1079443.278124999</v>
+        <v>1053103.853409091</v>
       </c>
       <c r="AB119" s="0">
-        <v>1045934.2812499991</v>
+        <v>1019132.7613636365</v>
       </c>
       <c r="AC119" s="0">
-        <v>0.009818707890134316</v>
+        <v>0.01096527789200804</v>
       </c>
     </row>
     <row r="120">
       <c r="B120" s="0">
-        <v>890412.6625000001</v>
+        <v>890283.9560344829</v>
       </c>
       <c r="C120" s="0">
-        <v>885413.4506944445</v>
+        <v>885282.3607758622</v>
       </c>
       <c r="D120" s="0">
-        <v>880414.238888889</v>
+        <v>880280.7655172416</v>
       </c>
       <c r="E120" s="0">
         <v>0.0008634697128170564</v>
       </c>
       <c r="H120" s="0">
-        <v>32769.452499999985</v>
+        <v>32594.23692307692</v>
       </c>
       <c r="I120" s="0">
-        <v>32343.82569444443</v>
+        <v>32165.365384615383</v>
       </c>
       <c r="J120" s="0">
-        <v>31918.198888888874</v>
+        <v>31736.493846153844</v>
       </c>
       <c r="K120" s="0">
-        <v>0.0002490535963339311</v>
+        <v>0.00014943215780035862</v>
       </c>
       <c r="N120" s="0">
         <v>-1147985.60625</v>
@@ -7433,42 +7433,42 @@
         <v>0.0009480839268561747</v>
       </c>
       <c r="Z120" s="0">
-        <v>1179970.2687499993</v>
+        <v>1155017.1295454546</v>
       </c>
       <c r="AA120" s="0">
-        <v>1146461.2718749994</v>
+        <v>1121046.0375</v>
       </c>
       <c r="AB120" s="0">
-        <v>1112952.2749999994</v>
+        <v>1087074.9454545456</v>
       </c>
       <c r="AC120" s="0">
-        <v>0.008736703458517655</v>
+        <v>0.009053557596856922</v>
       </c>
     </row>
     <row r="121">
       <c r="B121" s="0">
-        <v>900411.0861111111</v>
+        <v>900287.1465517243</v>
       </c>
       <c r="C121" s="0">
-        <v>895411.8743055555</v>
+        <v>895285.5512931036</v>
       </c>
       <c r="D121" s="0">
-        <v>890412.6625</v>
+        <v>890283.9560344829</v>
       </c>
       <c r="E121" s="0">
         <v>0.0004815455756753146</v>
       </c>
       <c r="H121" s="0">
-        <v>33620.706111111096</v>
+        <v>33451.979999999996</v>
       </c>
       <c r="I121" s="0">
-        <v>33195.07930555554</v>
+        <v>33023.10846153845</v>
       </c>
       <c r="J121" s="0">
-        <v>32769.452499999985</v>
+        <v>32594.236923076918</v>
       </c>
       <c r="K121" s="0">
-        <v>4.981071926678621E-05</v>
+        <v>9.962143853357243E-05</v>
       </c>
       <c r="N121" s="0">
         <v>-1147057.7652777778</v>
@@ -7495,42 +7495,42 @@
         <v>0.000898315269840085</v>
       </c>
       <c r="Z121" s="0">
-        <v>1246988.2624999988</v>
+        <v>1222959.3136363637</v>
       </c>
       <c r="AA121" s="0">
-        <v>1213479.2656249988</v>
+        <v>1188988.2215909092</v>
       </c>
       <c r="AB121" s="0">
-        <v>1179970.2687499989</v>
+        <v>1155017.1295454546</v>
       </c>
       <c r="AC121" s="0">
-        <v>0.008387356383027848</v>
+        <v>0.008786094192203367</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" s="0">
-        <v>910409.5097222223</v>
+        <v>910290.3370689657</v>
       </c>
       <c r="C122" s="0">
-        <v>905410.2979166667</v>
+        <v>905288.741810345</v>
       </c>
       <c r="D122" s="0">
-        <v>900411.0861111112</v>
+        <v>900287.1465517243</v>
       </c>
       <c r="E122" s="0">
         <v>0.0007140375550166979</v>
       </c>
       <c r="H122" s="0">
-        <v>34471.95972222221</v>
+        <v>34309.723076923074</v>
       </c>
       <c r="I122" s="0">
-        <v>34046.33291666665</v>
+        <v>33880.85153846153</v>
       </c>
       <c r="J122" s="0">
-        <v>33620.706111111096</v>
+        <v>33451.979999999996</v>
       </c>
       <c r="K122" s="0">
-        <v>9.962143853357243E-05</v>
+        <v>0.00014943215780035862</v>
       </c>
       <c r="N122" s="0">
         <v>-1146129.9243055556</v>
@@ -7557,39 +7557,39 @@
         <v>0.0008314388234982855</v>
       </c>
       <c r="Z122" s="0">
-        <v>1314006.2562499992</v>
+        <v>1290901.4977272728</v>
       </c>
       <c r="AA122" s="0">
-        <v>1280497.2593749992</v>
+        <v>1256930.4056818183</v>
       </c>
       <c r="AB122" s="0">
-        <v>1246988.2624999993</v>
+        <v>1222959.3136363637</v>
       </c>
       <c r="AC122" s="0">
-        <v>0.007888073039655217</v>
+        <v>0.008337335670970525</v>
       </c>
     </row>
     <row r="123">
       <c r="B123" s="0">
-        <v>920407.9333333333</v>
+        <v>920293.527586207</v>
       </c>
       <c r="C123" s="0">
-        <v>915408.7215277777</v>
+        <v>915291.9323275863</v>
       </c>
       <c r="D123" s="0">
-        <v>910409.5097222222</v>
+        <v>910290.3370689657</v>
       </c>
       <c r="E123" s="0">
         <v>0.0009796527683431763</v>
       </c>
       <c r="H123" s="0">
-        <v>35323.21333333332</v>
+        <v>35167.46615384615</v>
       </c>
       <c r="I123" s="0">
-        <v>34897.58652777776</v>
+        <v>34738.59461538461</v>
       </c>
       <c r="J123" s="0">
-        <v>34471.95972222221</v>
+        <v>34309.723076923074</v>
       </c>
       <c r="K123" s="0">
         <v>4.981071926678621E-05</v>
@@ -7619,39 +7619,39 @@
         <v>0.000581713186542049</v>
       </c>
       <c r="Z123" s="0">
-        <v>1381024.2499999995</v>
+        <v>1358843.6818181819</v>
       </c>
       <c r="AA123" s="0">
-        <v>1347515.2531249996</v>
+        <v>1324872.5897727273</v>
       </c>
       <c r="AB123" s="0">
-        <v>1314006.2562499996</v>
+        <v>1290901.4977272728</v>
       </c>
       <c r="AC123" s="0">
-        <v>0.00675646756309936</v>
+        <v>0.007106192880382489</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" s="0">
-        <v>930406.3569444444</v>
+        <v>930296.7181034484</v>
       </c>
       <c r="C124" s="0">
-        <v>925407.1451388887</v>
+        <v>925295.1228448277</v>
       </c>
       <c r="D124" s="0">
-        <v>920407.9333333332</v>
+        <v>920293.527586207</v>
       </c>
       <c r="E124" s="0">
         <v>0.0007140375550166979</v>
       </c>
       <c r="H124" s="0">
-        <v>36174.46694444443</v>
+        <v>36025.20923076923</v>
       </c>
       <c r="I124" s="0">
-        <v>35748.840138888874</v>
+        <v>35596.33769230769</v>
       </c>
       <c r="J124" s="0">
-        <v>35323.21333333332</v>
+        <v>35167.46615384615</v>
       </c>
       <c r="K124" s="0">
         <v>4.981071926678621E-05</v>
@@ -7681,39 +7681,39 @@
         <v>0.0004825117335895494</v>
       </c>
       <c r="Z124" s="0">
-        <v>1448042.243749999</v>
+        <v>1426785.865909091</v>
       </c>
       <c r="AA124" s="0">
-        <v>1414533.246874999</v>
+        <v>1392814.7738636364</v>
       </c>
       <c r="AB124" s="0">
-        <v>1381024.249999999</v>
+        <v>1358843.6818181819</v>
       </c>
       <c r="AC124" s="0">
-        <v>0.006057857218158194</v>
+        <v>0.006490390301941114</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" s="0">
-        <v>940404.7805555556</v>
+        <v>940299.9086206898</v>
       </c>
       <c r="C125" s="0">
-        <v>935405.56875</v>
+        <v>935298.3133620691</v>
       </c>
       <c r="D125" s="0">
-        <v>930406.3569444445</v>
+        <v>930296.7181034484</v>
       </c>
       <c r="E125" s="0">
-        <v>0.0007140375550166979</v>
+        <v>0.0006642268357499117</v>
       </c>
       <c r="H125" s="0">
-        <v>37025.72055555554</v>
+        <v>36882.95230769231</v>
       </c>
       <c r="I125" s="0">
-        <v>36600.093749999985</v>
+        <v>36454.080769230764</v>
       </c>
       <c r="J125" s="0">
-        <v>36174.46694444443</v>
+        <v>36025.20923076923</v>
       </c>
       <c r="K125" s="0">
         <v>9.962143853357243E-05</v>
@@ -7743,39 +7743,39 @@
         <v>0.0007316073921741767</v>
       </c>
       <c r="Z125" s="0">
-        <v>1515060.2374999993</v>
+        <v>1494728.05</v>
       </c>
       <c r="AA125" s="0">
-        <v>1481551.2406249994</v>
+        <v>1460756.9579545455</v>
       </c>
       <c r="AB125" s="0">
-        <v>1448042.2437499994</v>
+        <v>1426785.865909091</v>
       </c>
       <c r="AC125" s="0">
-        <v>0.005459372421833065</v>
+        <v>0.004976482446450196</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" s="0">
-        <v>950403.2041666666</v>
+        <v>950303.0991379311</v>
       </c>
       <c r="C126" s="0">
-        <v>945403.992361111</v>
+        <v>945301.5038793104</v>
       </c>
       <c r="D126" s="0">
-        <v>940404.7805555555</v>
+        <v>940299.9086206898</v>
       </c>
       <c r="E126" s="0">
-        <v>0.0006642268357499117</v>
+        <v>0.0007140375550166979</v>
       </c>
       <c r="H126" s="0">
-        <v>37876.97416666665</v>
+        <v>37740.695384615385</v>
       </c>
       <c r="I126" s="0">
-        <v>37451.3473611111</v>
+        <v>37311.82384615384</v>
       </c>
       <c r="J126" s="0">
-        <v>37025.72055555554</v>
+        <v>36882.95230769231</v>
       </c>
       <c r="K126" s="0">
         <v>0.0002490535963339311</v>
@@ -7805,39 +7805,39 @@
         <v>0.00044875852123284514</v>
       </c>
       <c r="Z126" s="0">
-        <v>1582078.2312499988</v>
+        <v>1562670.2340909091</v>
       </c>
       <c r="AA126" s="0">
-        <v>1548569.2343749988</v>
+        <v>1528699.1420454546</v>
       </c>
       <c r="AB126" s="0">
-        <v>1515060.2374999989</v>
+        <v>1494728.05</v>
       </c>
       <c r="AC126" s="0">
-        <v>0.005176313558101198</v>
+        <v>0.005742221292774395</v>
       </c>
     </row>
     <row r="127">
       <c r="B127" s="0">
-        <v>960401.6277777778</v>
+        <v>960306.2896551725</v>
       </c>
       <c r="C127" s="0">
-        <v>955402.4159722222</v>
+        <v>955304.6943965518</v>
       </c>
       <c r="D127" s="0">
-        <v>950403.2041666667</v>
+        <v>950303.0991379311</v>
       </c>
       <c r="E127" s="0">
         <v>0.001545139243583518</v>
       </c>
       <c r="H127" s="0">
-        <v>38728.22777777776</v>
+        <v>38598.438461538455</v>
       </c>
       <c r="I127" s="0">
-        <v>38302.60097222221</v>
+        <v>38169.56692307691</v>
       </c>
       <c r="J127" s="0">
-        <v>37876.97416666665</v>
+        <v>37740.69538461538</v>
       </c>
       <c r="K127" s="0">
         <v>4.981071926678621E-05</v>
@@ -7867,39 +7867,39 @@
         <v>0.0005989047819062057</v>
       </c>
       <c r="Z127" s="0">
-        <v>1649096.2249999992</v>
+        <v>1630612.4181818182</v>
       </c>
       <c r="AA127" s="0">
-        <v>1615587.2281249992</v>
+        <v>1596641.3261363637</v>
       </c>
       <c r="AB127" s="0">
-        <v>1582078.2312499993</v>
+        <v>1562670.2340909091</v>
       </c>
       <c r="AC127" s="0">
-        <v>0.004759921787266807</v>
+        <v>0.004810110748326915</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" s="0">
-        <v>970400.0513888889</v>
+        <v>970309.4801724139</v>
       </c>
       <c r="C128" s="0">
-        <v>965400.8395833332</v>
+        <v>965307.8849137932</v>
       </c>
       <c r="D128" s="0">
-        <v>960401.6277777777</v>
+        <v>960306.2896551725</v>
       </c>
       <c r="E128" s="0">
-        <v>0.003407214839230018</v>
+        <v>0.003340716634681541</v>
       </c>
       <c r="H128" s="0">
-        <v>39579.481388888875</v>
+        <v>39456.18153846153</v>
       </c>
       <c r="I128" s="0">
-        <v>39153.85458333332</v>
+        <v>39027.30999999999</v>
       </c>
       <c r="J128" s="0">
-        <v>38728.22777777776</v>
+        <v>38598.438461538455</v>
       </c>
       <c r="K128" s="0">
         <v>0.00014943215780035862</v>
@@ -7929,39 +7929,39 @@
         <v>0.00019945286985768117</v>
       </c>
       <c r="Z128" s="0">
-        <v>1716114.2187499995</v>
+        <v>1698554.6022727275</v>
       </c>
       <c r="AA128" s="0">
-        <v>1682605.2218749996</v>
+        <v>1664583.510227273</v>
       </c>
       <c r="AB128" s="0">
-        <v>1649096.2249999996</v>
+        <v>1630612.4181818184</v>
       </c>
       <c r="AC128" s="0">
-        <v>0.004975515333147125</v>
+        <v>0.005324988595389021</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" s="0">
-        <v>980398.4750000001</v>
+        <v>980312.6706896554</v>
       </c>
       <c r="C129" s="0">
-        <v>975399.2631944445</v>
+        <v>975311.0754310347</v>
       </c>
       <c r="D129" s="0">
-        <v>970400.051388889</v>
+        <v>970309.480172414</v>
       </c>
       <c r="E129" s="0">
         <v>0.006981304531276943</v>
       </c>
       <c r="H129" s="0">
-        <v>40430.734999999986</v>
+        <v>40313.92461538461</v>
       </c>
       <c r="I129" s="0">
-        <v>40005.10819444443</v>
+        <v>39885.05307692307</v>
       </c>
       <c r="J129" s="0">
-        <v>39579.481388888875</v>
+        <v>39456.18153846153</v>
       </c>
       <c r="K129" s="0">
         <v>0</v>
@@ -7991,39 +7991,39 @@
         <v>0.00014964215059089497</v>
       </c>
       <c r="Z129" s="0">
-        <v>1783132.212499999</v>
+        <v>1766496.7863636366</v>
       </c>
       <c r="AA129" s="0">
-        <v>1749623.215624999</v>
+        <v>1732525.694318182</v>
       </c>
       <c r="AB129" s="0">
-        <v>1716114.218749999</v>
+        <v>1698554.6022727275</v>
       </c>
       <c r="AC129" s="0">
-        <v>0.003295362921673851</v>
+        <v>0.003644793803202105</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" s="0">
-        <v>990396.8986111111</v>
+        <v>990315.8612068967</v>
       </c>
       <c r="C130" s="0">
-        <v>985397.6868055555</v>
+        <v>985314.265948276</v>
       </c>
       <c r="D130" s="0">
-        <v>980398.475</v>
+        <v>980312.6706896554</v>
       </c>
       <c r="E130" s="0">
-        <v>0.0038886345466161883</v>
+        <v>0.003955132751164665</v>
       </c>
       <c r="H130" s="0">
-        <v>41281.9886111111</v>
+        <v>41171.66769230769</v>
       </c>
       <c r="I130" s="0">
-        <v>40856.36180555554</v>
+        <v>40742.796153846146</v>
       </c>
       <c r="J130" s="0">
-        <v>40430.734999999986</v>
+        <v>40313.92461538461</v>
       </c>
       <c r="K130" s="0">
         <v>9.962143853357243E-05</v>
@@ -8053,39 +8053,39 @@
         <v>0.0002492215268737709</v>
       </c>
       <c r="Z130" s="0">
-        <v>1850150.2062499984</v>
+        <v>1834438.9704545457</v>
       </c>
       <c r="AA130" s="0">
-        <v>1816641.2093749985</v>
+        <v>1800467.8784090912</v>
       </c>
       <c r="AB130" s="0">
-        <v>1783132.2124999985</v>
+        <v>1766496.7863636366</v>
       </c>
       <c r="AC130" s="0">
-        <v>0.0027794341552702263</v>
+        <v>0.0030289918616866218</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" s="0">
-        <v>1000395.3222222223</v>
+        <v>1000319.0517241381</v>
       </c>
       <c r="C131" s="0">
-        <v>995396.1104166667</v>
+        <v>995317.4564655174</v>
       </c>
       <c r="D131" s="0">
-        <v>990396.8986111112</v>
+        <v>990315.8612068967</v>
       </c>
       <c r="E131" s="0">
         <v>0.00152820002172354</v>
       </c>
       <c r="H131" s="0">
-        <v>42133.24222222221</v>
+        <v>42029.410769230766</v>
       </c>
       <c r="I131" s="0">
-        <v>41707.61541666665</v>
+        <v>41600.539230769224</v>
       </c>
       <c r="J131" s="0">
-        <v>41281.9886111111</v>
+        <v>41171.66769230769</v>
       </c>
       <c r="K131" s="0">
         <v>4.981071926678621E-05</v>
@@ -8115,39 +8115,39 @@
         <v>8.305982154102482E-05</v>
       </c>
       <c r="Z131" s="0">
-        <v>1917168.1999999988</v>
+        <v>1902381.1545454548</v>
       </c>
       <c r="AA131" s="0">
-        <v>1883659.2031249988</v>
+        <v>1868410.0625000002</v>
       </c>
       <c r="AB131" s="0">
-        <v>1850150.2062499989</v>
+        <v>1834438.9704545457</v>
       </c>
       <c r="AC131" s="0">
-        <v>0.00231360990696237</v>
+        <v>0.0024134834005371747</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" s="0">
-        <v>1010393.7458333333</v>
+        <v>1010322.2422413795</v>
       </c>
       <c r="C132" s="0">
-        <v>1005394.5340277777</v>
+        <v>1005320.6469827588</v>
       </c>
       <c r="D132" s="0">
-        <v>1000395.3222222222</v>
+        <v>1000319.0517241381</v>
       </c>
       <c r="E132" s="0">
         <v>0.000747160789001793</v>
       </c>
       <c r="H132" s="0">
-        <v>42984.49583333332</v>
+        <v>42887.153846153844</v>
       </c>
       <c r="I132" s="0">
-        <v>42558.869027777764</v>
+        <v>42458.2823076923</v>
       </c>
       <c r="J132" s="0">
-        <v>42133.24222222221</v>
+        <v>42029.410769230766</v>
       </c>
       <c r="K132" s="0">
         <v>0</v>
@@ -8177,39 +8177,39 @@
         <v>0.00011630892381526341</v>
       </c>
       <c r="Z132" s="0">
-        <v>1984186.1937499992</v>
+        <v>1970323.3386363639</v>
       </c>
       <c r="AA132" s="0">
-        <v>1950677.1968749992</v>
+        <v>1936352.2465909093</v>
       </c>
       <c r="AB132" s="0">
-        <v>1917168.1999999993</v>
+        <v>1902381.1545454548</v>
       </c>
       <c r="AC132" s="0">
-        <v>0.0010653172647979226</v>
+        <v>0.0014648112390971437</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" s="0">
-        <v>1020392.1694444444</v>
+        <v>1020325.4327586208</v>
       </c>
       <c r="C133" s="0">
-        <v>1015392.9576388887</v>
+        <v>1015323.8375000001</v>
       </c>
       <c r="D133" s="0">
-        <v>1010393.7458333332</v>
+        <v>1010322.2422413795</v>
       </c>
       <c r="E133" s="0">
         <v>0.0006973500697350068</v>
       </c>
       <c r="H133" s="0">
-        <v>43835.74944444443</v>
+        <v>43744.89692307692</v>
       </c>
       <c r="I133" s="0">
-        <v>43410.122638888875</v>
+        <v>43316.02538461538</v>
       </c>
       <c r="J133" s="0">
-        <v>42984.49583333332</v>
+        <v>42887.153846153844</v>
       </c>
       <c r="K133" s="0">
         <v>0</v>
@@ -8239,13 +8239,13 @@
         <v>0.0002159303623488358</v>
       </c>
       <c r="Z133" s="0">
-        <v>2051204.1874999995</v>
+        <v>2038265.522727273</v>
       </c>
       <c r="AA133" s="0">
-        <v>2017695.1906249996</v>
+        <v>2004294.4306818184</v>
       </c>
       <c r="AB133" s="0">
-        <v>1984186.1937499996</v>
+        <v>1970323.3386363639</v>
       </c>
       <c r="AC133" s="0">
         <v>0.0013316465809974033</v>
@@ -8253,28 +8253,28 @@
     </row>
     <row r="134">
       <c r="B134" s="0">
-        <v>1030390.5930555556</v>
+        <v>1030328.6232758622</v>
       </c>
       <c r="C134" s="0">
-        <v>1025391.38125</v>
+        <v>1025327.0280172415</v>
       </c>
       <c r="D134" s="0">
-        <v>1020392.1694444445</v>
+        <v>1020325.4327586208</v>
       </c>
       <c r="E134" s="0">
         <v>0.0007969715082685792</v>
       </c>
       <c r="H134" s="0">
-        <v>44687.00305555554</v>
+        <v>44602.64</v>
       </c>
       <c r="I134" s="0">
-        <v>44261.37624999999</v>
+        <v>44173.76846153846</v>
       </c>
       <c r="J134" s="0">
-        <v>43835.74944444443</v>
+        <v>43744.89692307692</v>
       </c>
       <c r="K134" s="0">
-        <v>9.962143853357243E-05</v>
+        <v>4.981071926678621E-05</v>
       </c>
       <c r="N134" s="0">
         <v>-1134995.8326388889</v>
@@ -8289,54 +8289,54 @@
         <v>4.981071926678621E-05</v>
       </c>
       <c r="T134" s="0">
-        <v>32361.09097222243</v>
+        <v>0</v>
       </c>
       <c r="U134" s="0">
-        <v>-5631.909374999792</v>
+        <v>-21812.454861110986</v>
       </c>
       <c r="V134" s="0">
-        <v>-43624.909722222015</v>
+        <v>-43624.90972222197</v>
       </c>
       <c r="W134" s="0">
         <v>8.305982154102482E-05</v>
       </c>
       <c r="Z134" s="0">
-        <v>2118222.18125</v>
+        <v>2106207.706818182</v>
       </c>
       <c r="AA134" s="0">
-        <v>2084713.184375</v>
+        <v>2072236.6147727275</v>
       </c>
       <c r="AB134" s="0">
-        <v>2051204.1875</v>
+        <v>2038265.522727273</v>
       </c>
       <c r="AC134" s="0">
-        <v>0.0009987349357480524</v>
+        <v>0.0010320261002729875</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" s="0">
-        <v>1040389.0166666666</v>
+        <v>1040331.8137931036</v>
       </c>
       <c r="C135" s="0">
-        <v>1035389.804861111</v>
+        <v>1035330.2185344829</v>
       </c>
       <c r="D135" s="0">
-        <v>1030390.5930555555</v>
+        <v>1030328.6232758622</v>
       </c>
       <c r="E135" s="0">
         <v>0.000448296473401076</v>
       </c>
       <c r="H135" s="0">
-        <v>45538.25666666665</v>
+        <v>45460.38307692308</v>
       </c>
       <c r="I135" s="0">
-        <v>45112.6298611111</v>
+        <v>45031.511538461535</v>
       </c>
       <c r="J135" s="0">
-        <v>44687.00305555554</v>
+        <v>44602.64</v>
       </c>
       <c r="K135" s="0">
-        <v>0</v>
+        <v>4.981071926678621E-05</v>
       </c>
       <c r="N135" s="0">
         <v>-1134067.9916666667</v>
@@ -8351,51 +8351,51 @@
         <v>0.00019924287706714485</v>
       </c>
       <c r="T135" s="0">
-        <v>108347.09166666683</v>
+        <v>78475.31538461539</v>
       </c>
       <c r="U135" s="0">
-        <v>70354.09131944462</v>
+        <v>39237.657692307694</v>
       </c>
       <c r="V135" s="0">
-        <v>32361.090972222388</v>
+        <v>0</v>
       </c>
       <c r="W135" s="0">
-        <v>0.00028242856689731304</v>
+        <v>0.0002491794646230744</v>
       </c>
       <c r="Z135" s="0">
-        <v>2185240.1749999984</v>
+        <v>2174149.890909091</v>
       </c>
       <c r="AA135" s="0">
-        <v>2151731.1781249987</v>
+        <v>2140178.798863637</v>
       </c>
       <c r="AB135" s="0">
-        <v>2118222.1812499985</v>
+        <v>2106207.706818182</v>
       </c>
       <c r="AC135" s="0">
-        <v>0.000798987948598442</v>
+        <v>0.0008655702776483122</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" s="0">
-        <v>1050387.4402777778</v>
+        <v>1050335.004310345</v>
       </c>
       <c r="C136" s="0">
-        <v>1045388.2284722222</v>
+        <v>1045333.4090517242</v>
       </c>
       <c r="D136" s="0">
-        <v>1040389.0166666667</v>
+        <v>1040331.8137931036</v>
       </c>
       <c r="E136" s="0">
         <v>0.0008965929468021515</v>
       </c>
       <c r="H136" s="0">
-        <v>46389.510277777765</v>
+        <v>46318.12615384615</v>
       </c>
       <c r="I136" s="0">
-        <v>45963.88347222221</v>
+        <v>45889.254615384605</v>
       </c>
       <c r="J136" s="0">
-        <v>45538.25666666665</v>
+        <v>45460.38307692307</v>
       </c>
       <c r="K136" s="0">
         <v>9.962143853357243E-05</v>
@@ -8413,51 +8413,51 @@
         <v>9.962143853357243E-05</v>
       </c>
       <c r="T136" s="0">
-        <v>184333.09236111125</v>
+        <v>156950.63076923077</v>
       </c>
       <c r="U136" s="0">
-        <v>146340.09201388902</v>
+        <v>117712.97307692308</v>
       </c>
       <c r="V136" s="0">
-        <v>108347.09166666679</v>
+        <v>78475.31538461539</v>
       </c>
       <c r="W136" s="0">
-        <v>9.97473068227158E-05</v>
+        <v>6.64982045484772E-05</v>
       </c>
       <c r="Z136" s="0">
-        <v>2252258.168749999</v>
+        <v>2242092.075</v>
       </c>
       <c r="AA136" s="0">
-        <v>2218749.171874999</v>
+        <v>2208120.982954546</v>
       </c>
       <c r="AB136" s="0">
-        <v>2185240.174999999</v>
+        <v>2174149.890909091</v>
       </c>
       <c r="AC136" s="0">
-        <v>0.0007987358935572091</v>
+        <v>0.0007156340097654878</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" s="0">
-        <v>1060385.8638888886</v>
+        <v>1060338.1948275864</v>
       </c>
       <c r="C137" s="0">
-        <v>1055386.652083333</v>
+        <v>1055336.5995689658</v>
       </c>
       <c r="D137" s="0">
-        <v>1050387.4402777776</v>
+        <v>1050335.004310345</v>
       </c>
       <c r="E137" s="0">
         <v>0.00034867503486750353</v>
       </c>
       <c r="H137" s="0">
-        <v>47240.763888888876</v>
+        <v>47175.869230769225</v>
       </c>
       <c r="I137" s="0">
-        <v>46815.13708333332</v>
+        <v>46746.99769230768</v>
       </c>
       <c r="J137" s="0">
-        <v>46389.510277777765</v>
+        <v>46318.12615384615</v>
       </c>
       <c r="K137" s="0">
         <v>4.981071926678621E-05</v>
@@ -8475,54 +8475,54 @@
         <v>4.981071926678621E-05</v>
       </c>
       <c r="T137" s="0">
-        <v>260319.09305555566</v>
+        <v>235425.94615384616</v>
       </c>
       <c r="U137" s="0">
-        <v>222326.09270833342</v>
+        <v>196188.28846153847</v>
       </c>
       <c r="V137" s="0">
-        <v>184333.0923611112</v>
+        <v>156950.63076923077</v>
       </c>
       <c r="W137" s="0">
-        <v>0.0001661196430820496</v>
+        <v>0.0001993687453562882</v>
       </c>
       <c r="Z137" s="0">
-        <v>2319276.162499999</v>
+        <v>2310034.2590909093</v>
       </c>
       <c r="AA137" s="0">
-        <v>2285767.1656249994</v>
+        <v>2276063.167045455</v>
       </c>
       <c r="AB137" s="0">
-        <v>2252258.1687499993</v>
+        <v>2242092.075</v>
       </c>
       <c r="AC137" s="0">
-        <v>0.0006658232904987017</v>
+        <v>0.0007489251742904229</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" s="0">
-        <v>1070384.2875</v>
+        <v>1070341.3853448278</v>
       </c>
       <c r="C138" s="0">
-        <v>1065385.0756944446</v>
+        <v>1065339.7900862072</v>
       </c>
       <c r="D138" s="0">
-        <v>1060385.863888889</v>
+        <v>1060338.1948275864</v>
       </c>
       <c r="E138" s="0">
         <v>0.0004981071926678622</v>
       </c>
       <c r="H138" s="0">
-        <v>48092.01749999999</v>
+        <v>48033.6123076923</v>
       </c>
       <c r="I138" s="0">
-        <v>47666.39069444443</v>
+        <v>47604.74076923076</v>
       </c>
       <c r="J138" s="0">
-        <v>47240.763888888876</v>
+        <v>47175.869230769225</v>
       </c>
       <c r="K138" s="0">
-        <v>4.981071926678621E-05</v>
+        <v>0</v>
       </c>
       <c r="N138" s="0">
         <v>-1131284.46875</v>
@@ -8537,54 +8537,54 @@
         <v>0.00019924287706714485</v>
       </c>
       <c r="T138" s="0">
-        <v>336305.09375000006</v>
+        <v>313901.26153846155</v>
       </c>
       <c r="U138" s="0">
-        <v>298312.0934027778</v>
+        <v>274663.6038461538</v>
       </c>
       <c r="V138" s="0">
-        <v>260319.0930555556</v>
+        <v>235425.94615384616</v>
       </c>
       <c r="W138" s="0">
         <v>0.0001993687453562882</v>
       </c>
       <c r="Z138" s="0">
-        <v>2386294.1562499995</v>
+        <v>2377976.4431818184</v>
       </c>
       <c r="AA138" s="0">
-        <v>2352785.159375</v>
+        <v>2344005.351136364</v>
       </c>
       <c r="AB138" s="0">
-        <v>2319276.1624999996</v>
+        <v>2310034.2590909093</v>
       </c>
       <c r="AC138" s="0">
-        <v>0.0005491781871408124</v>
+        <v>0.0004327851388241561</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" s="0">
-        <v>1080382.711111111</v>
+        <v>1080344.5758620691</v>
       </c>
       <c r="C139" s="0">
-        <v>1075383.4993055556</v>
+        <v>1075342.9806034486</v>
       </c>
       <c r="D139" s="0">
-        <v>1070384.2875</v>
+        <v>1070341.3853448278</v>
       </c>
       <c r="E139" s="0">
         <v>0.000448296473401076</v>
       </c>
       <c r="H139" s="0">
-        <v>48943.2711111111</v>
+        <v>48891.35538461538</v>
       </c>
       <c r="I139" s="0">
-        <v>48517.64430555554</v>
+        <v>48462.48384615384</v>
       </c>
       <c r="J139" s="0">
-        <v>48092.01749999999</v>
+        <v>48033.6123076923</v>
       </c>
       <c r="K139" s="0">
-        <v>0</v>
+        <v>4.981071926678621E-05</v>
       </c>
       <c r="N139" s="0">
         <v>-1130356.6277777778</v>
@@ -8599,51 +8599,51 @@
         <v>4.981071926678621E-05</v>
       </c>
       <c r="T139" s="0">
-        <v>412291.09444444446</v>
+        <v>392376.57692307694</v>
       </c>
       <c r="U139" s="0">
-        <v>374298.0940972222</v>
+        <v>353138.9192307693</v>
       </c>
       <c r="V139" s="0">
-        <v>336305.09375</v>
+        <v>313901.26153846155</v>
       </c>
       <c r="W139" s="0">
         <v>0.0001828071283637406</v>
       </c>
       <c r="Z139" s="0">
-        <v>2453312.15</v>
+        <v>2445918.6272727274</v>
       </c>
       <c r="AA139" s="0">
-        <v>2419803.153125</v>
+        <v>2411947.535227273</v>
       </c>
       <c r="AB139" s="0">
-        <v>2386294.15625</v>
+        <v>2377976.4431818184</v>
       </c>
       <c r="AC139" s="0">
-        <v>0.0004825958580909423</v>
+        <v>0.0005989889064075986</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" s="0">
-        <v>1090381.134722222</v>
+        <v>1090347.7663793105</v>
       </c>
       <c r="C140" s="0">
-        <v>1085381.9229166666</v>
+        <v>1085346.17112069</v>
       </c>
       <c r="D140" s="0">
-        <v>1080382.711111111</v>
+        <v>1080344.5758620691</v>
       </c>
       <c r="E140" s="0">
         <v>0.0012950787009364416</v>
       </c>
       <c r="H140" s="0">
-        <v>49794.52472222221</v>
+        <v>49749.09846153846</v>
       </c>
       <c r="I140" s="0">
-        <v>49368.897916666654</v>
+        <v>49320.226923076916</v>
       </c>
       <c r="J140" s="0">
-        <v>48943.2711111111</v>
+        <v>48891.35538461538</v>
       </c>
       <c r="K140" s="0">
         <v>4.981071926678621E-05</v>
@@ -8661,51 +8661,51 @@
         <v>0</v>
       </c>
       <c r="T140" s="0">
-        <v>488277.09513888886</v>
+        <v>470851.8923076923</v>
       </c>
       <c r="U140" s="0">
-        <v>450284.0947916666</v>
+        <v>431614.2346153846</v>
       </c>
       <c r="V140" s="0">
-        <v>412291.0944444444</v>
+        <v>392376.57692307694</v>
       </c>
       <c r="W140" s="0">
-        <v>0.0001329964090969544</v>
+        <v>9.97473068227158E-05</v>
       </c>
       <c r="Z140" s="0">
-        <v>2520330.1437499984</v>
+        <v>2513860.8113636365</v>
       </c>
       <c r="AA140" s="0">
-        <v>2486821.1468749987</v>
+        <v>2479889.719318182</v>
       </c>
       <c r="AB140" s="0">
-        <v>2453312.1499999985</v>
+        <v>2445918.6272727274</v>
       </c>
       <c r="AC140" s="0">
-        <v>0.00038272236451613705</v>
+        <v>0.00044930469356600723</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" s="0">
-        <v>1100379.558333333</v>
+        <v>1100350.956896552</v>
       </c>
       <c r="C141" s="0">
-        <v>1095380.3465277776</v>
+        <v>1095349.3616379313</v>
       </c>
       <c r="D141" s="0">
-        <v>1090381.134722222</v>
+        <v>1090347.7663793105</v>
       </c>
       <c r="E141" s="0">
         <v>0.0005479179119346483</v>
       </c>
       <c r="H141" s="0">
-        <v>50645.77833333332</v>
+        <v>50606.84153846154</v>
       </c>
       <c r="I141" s="0">
-        <v>50220.151527777765</v>
+        <v>50177.969999999994</v>
       </c>
       <c r="J141" s="0">
-        <v>49794.52472222221</v>
+        <v>49749.09846153846</v>
       </c>
       <c r="K141" s="0">
         <v>4.981071926678621E-05</v>
@@ -8723,25 +8723,25 @@
         <v>0.0002490535963339311</v>
       </c>
       <c r="T141" s="0">
-        <v>564263.0958333332</v>
+        <v>549327.2076923077</v>
       </c>
       <c r="U141" s="0">
-        <v>526270.095486111</v>
+        <v>510089.55000000005</v>
       </c>
       <c r="V141" s="0">
-        <v>488277.0951388888</v>
+        <v>470851.8923076923</v>
       </c>
       <c r="W141" s="0">
-        <v>9.97473068227158E-05</v>
+        <v>0.00016624551137119298</v>
       </c>
       <c r="Z141" s="0">
-        <v>2587348.137499999</v>
+        <v>2581802.9954545456</v>
       </c>
       <c r="AA141" s="0">
-        <v>2553839.140624999</v>
+        <v>2547831.9034090913</v>
       </c>
       <c r="AB141" s="0">
-        <v>2520330.143749999</v>
+        <v>2513860.8113636365</v>
       </c>
       <c r="AC141" s="0">
         <v>0.0002330381516745456</v>
@@ -8749,25 +8749,25 @@
     </row>
     <row r="142">
       <c r="B142" s="0">
-        <v>1110377.9819444441</v>
+        <v>1110354.1474137933</v>
       </c>
       <c r="C142" s="0">
-        <v>1105378.7701388886</v>
+        <v>1105352.5521551727</v>
       </c>
       <c r="D142" s="0">
-        <v>1100379.558333333</v>
+        <v>1100350.956896552</v>
       </c>
       <c r="E142" s="0">
         <v>0.0006973500697350068</v>
       </c>
       <c r="H142" s="0">
-        <v>51497.03194444443</v>
+        <v>51464.584615384614</v>
       </c>
       <c r="I142" s="0">
-        <v>51071.40513888888</v>
+        <v>51035.71307692307</v>
       </c>
       <c r="J142" s="0">
-        <v>50645.77833333332</v>
+        <v>50606.84153846154</v>
       </c>
       <c r="K142" s="0">
         <v>0</v>
@@ -8785,25 +8785,25 @@
         <v>9.962143853357243E-05</v>
       </c>
       <c r="T142" s="0">
-        <v>640249.0965277776</v>
+        <v>627802.5230769231</v>
       </c>
       <c r="U142" s="0">
-        <v>602256.0961805554</v>
+        <v>588564.8653846154</v>
       </c>
       <c r="V142" s="0">
-        <v>564263.0958333332</v>
+        <v>549327.2076923077</v>
       </c>
       <c r="W142" s="0">
-        <v>0.0002326178476305268</v>
+        <v>6.64982045484772E-05</v>
       </c>
       <c r="Z142" s="0">
-        <v>2654366.131249999</v>
+        <v>2649745.1795454547</v>
       </c>
       <c r="AA142" s="0">
-        <v>2620857.1343749994</v>
+        <v>2615774.0875000004</v>
       </c>
       <c r="AB142" s="0">
-        <v>2587348.1374999993</v>
+        <v>2581802.9954545456</v>
       </c>
       <c r="AC142" s="0">
         <v>0.0001997469871496105</v>
@@ -8811,25 +8811,25 @@
     </row>
     <row r="143">
       <c r="B143" s="0">
-        <v>1120376.4055555556</v>
+        <v>1120357.3379310346</v>
       </c>
       <c r="C143" s="0">
-        <v>1115377.19375</v>
+        <v>1115355.742672414</v>
       </c>
       <c r="D143" s="0">
-        <v>1110377.9819444446</v>
+        <v>1110354.1474137933</v>
       </c>
       <c r="E143" s="0">
         <v>0.000448296473401076</v>
       </c>
       <c r="H143" s="0">
-        <v>52348.28555555554</v>
+        <v>52322.327692307685</v>
       </c>
       <c r="I143" s="0">
-        <v>51922.65874999999</v>
+        <v>51893.45615384614</v>
       </c>
       <c r="J143" s="0">
-        <v>51497.03194444443</v>
+        <v>51464.58461538461</v>
       </c>
       <c r="K143" s="0">
         <v>4.981071926678621E-05</v>
@@ -8847,25 +8847,25 @@
         <v>4.981071926678621E-05</v>
       </c>
       <c r="T143" s="0">
-        <v>716235.097222222</v>
+        <v>706277.8384615385</v>
       </c>
       <c r="U143" s="0">
-        <v>678242.0968749998</v>
+        <v>667040.1807692308</v>
       </c>
       <c r="V143" s="0">
-        <v>640249.0965277776</v>
+        <v>627802.5230769231</v>
       </c>
       <c r="W143" s="0">
-        <v>6.64982045484772E-05</v>
+        <v>0.0002326178476305268</v>
       </c>
       <c r="Z143" s="0">
-        <v>2721384.1249999995</v>
+        <v>2717687.3636363638</v>
       </c>
       <c r="AA143" s="0">
-        <v>2687875.128125</v>
+        <v>2683716.2715909095</v>
       </c>
       <c r="AB143" s="0">
-        <v>2654366.1312499996</v>
+        <v>2649745.1795454547</v>
       </c>
       <c r="AC143" s="0">
         <v>0.00013316465809974033</v>
@@ -8873,25 +8873,25 @@
     </row>
     <row r="144">
       <c r="B144" s="0">
-        <v>1130374.8291666666</v>
+        <v>1130360.528448276</v>
       </c>
       <c r="C144" s="0">
-        <v>1125375.617361111</v>
+        <v>1125358.9331896554</v>
       </c>
       <c r="D144" s="0">
-        <v>1120376.4055555556</v>
+        <v>1120357.3379310346</v>
       </c>
       <c r="E144" s="0">
         <v>0.0002490535963339311</v>
       </c>
       <c r="H144" s="0">
-        <v>53199.539166666655</v>
+        <v>53180.07076923076</v>
       </c>
       <c r="I144" s="0">
-        <v>52773.9123611111</v>
+        <v>52751.19923076922</v>
       </c>
       <c r="J144" s="0">
-        <v>52348.28555555554</v>
+        <v>52322.327692307685</v>
       </c>
       <c r="K144" s="0">
         <v>4.981071926678621E-05</v>
@@ -8909,25 +8909,25 @@
         <v>9.962143853357243E-05</v>
       </c>
       <c r="T144" s="0">
-        <v>792221.0979166664</v>
+        <v>784753.153846154</v>
       </c>
       <c r="U144" s="0">
-        <v>754228.0975694442</v>
+        <v>745515.4961538463</v>
       </c>
       <c r="V144" s="0">
-        <v>716235.097222222</v>
+        <v>706277.8384615385</v>
       </c>
       <c r="W144" s="0">
         <v>0.0001329964090969544</v>
       </c>
       <c r="Z144" s="0">
-        <v>2788402.11875</v>
+        <v>2785629.547727273</v>
       </c>
       <c r="AA144" s="0">
-        <v>2754893.121875</v>
+        <v>2751658.4556818185</v>
       </c>
       <c r="AB144" s="0">
-        <v>2721384.125</v>
+        <v>2717687.3636363638</v>
       </c>
       <c r="AC144" s="0">
         <v>0.00011639304831665638</v>
@@ -8935,25 +8935,25 @@
     </row>
     <row r="145">
       <c r="B145" s="0">
-        <v>1140373.2527777776</v>
+        <v>1140363.7189655174</v>
       </c>
       <c r="C145" s="0">
-        <v>1135374.040972222</v>
+        <v>1135362.1237068968</v>
       </c>
       <c r="D145" s="0">
-        <v>1130374.8291666666</v>
+        <v>1130360.528448276</v>
       </c>
       <c r="E145" s="0">
         <v>0.00019924287706714485</v>
       </c>
       <c r="H145" s="0">
-        <v>54050.792777777766</v>
+        <v>54037.81384615384</v>
       </c>
       <c r="I145" s="0">
-        <v>53625.16597222221</v>
+        <v>53608.9423076923</v>
       </c>
       <c r="J145" s="0">
-        <v>53199.539166666655</v>
+        <v>53180.07076923076</v>
       </c>
       <c r="K145" s="0">
         <v>0</v>
@@ -8971,25 +8971,25 @@
         <v>9.962143853357243E-05</v>
       </c>
       <c r="T145" s="0">
-        <v>868207.0986111108</v>
+        <v>863228.4692307692</v>
       </c>
       <c r="U145" s="0">
-        <v>830214.0982638886</v>
+        <v>823990.8115384616</v>
       </c>
       <c r="V145" s="0">
-        <v>792221.0979166664</v>
+        <v>784753.1538461539</v>
       </c>
       <c r="W145" s="0">
         <v>0.0001329964090969544</v>
       </c>
       <c r="Z145" s="0">
-        <v>2855420.1124999984</v>
+        <v>2853571.731818182</v>
       </c>
       <c r="AA145" s="0">
-        <v>2821911.1156249987</v>
+        <v>2819600.6397727276</v>
       </c>
       <c r="AB145" s="0">
-        <v>2788402.1187499985</v>
+        <v>2785629.547727273</v>
       </c>
       <c r="AC145" s="0">
         <v>0.0002330381516745456</v>
@@ -8997,25 +8997,25 @@
     </row>
     <row r="146">
       <c r="B146" s="0">
-        <v>1150371.6763888886</v>
+        <v>1150366.9094827587</v>
       </c>
       <c r="C146" s="0">
-        <v>1145372.464583333</v>
+        <v>1145365.3142241382</v>
       </c>
       <c r="D146" s="0">
-        <v>1140373.2527777776</v>
+        <v>1140363.7189655174</v>
       </c>
       <c r="E146" s="0">
         <v>0.0002988643156007173</v>
       </c>
       <c r="H146" s="0">
-        <v>54902.04638888888</v>
+        <v>54895.55692307692</v>
       </c>
       <c r="I146" s="0">
-        <v>54476.41958333332</v>
+        <v>54466.685384615375</v>
       </c>
       <c r="J146" s="0">
-        <v>54050.792777777766</v>
+        <v>54037.81384615384</v>
       </c>
       <c r="K146" s="0">
         <v>4.981071926678621E-05</v>
@@ -9033,25 +9033,25 @@
         <v>0.00014943215780035862</v>
       </c>
       <c r="T146" s="0">
-        <v>944193.0993055552</v>
+        <v>941703.7846153846</v>
       </c>
       <c r="U146" s="0">
-        <v>906200.098958333</v>
+        <v>902466.1269230769</v>
       </c>
       <c r="V146" s="0">
-        <v>868207.0986111108</v>
+        <v>863228.4692307692</v>
       </c>
       <c r="W146" s="0">
-        <v>0.00016624551137119298</v>
+        <v>0.0001329964090969544</v>
       </c>
       <c r="Z146" s="0">
-        <v>2922438.106249999</v>
+        <v>2921513.915909091</v>
       </c>
       <c r="AA146" s="0">
-        <v>2888929.109374999</v>
+        <v>2887542.8238636367</v>
       </c>
       <c r="AB146" s="0">
-        <v>2855420.112499999</v>
+        <v>2853571.731818182</v>
       </c>
       <c r="AC146" s="0">
         <v>9.987349357480524E-05</v>
@@ -9062,22 +9062,22 @@
         <v>1160370.1</v>
       </c>
       <c r="C147" s="0">
-        <v>1155370.8881944446</v>
+        <v>1155368.5047413795</v>
       </c>
       <c r="D147" s="0">
-        <v>1150371.676388889</v>
+        <v>1150366.9094827587</v>
       </c>
       <c r="E147" s="0">
         <v>4.981071926678621E-05</v>
       </c>
       <c r="H147" s="0">
-        <v>55753.29999999999</v>
+        <v>55753.299999999996</v>
       </c>
       <c r="I147" s="0">
-        <v>55327.67319444443</v>
+        <v>55324.42846153845</v>
       </c>
       <c r="J147" s="0">
-        <v>54902.04638888888</v>
+        <v>54895.55692307692</v>
       </c>
       <c r="K147" s="0">
         <v>4.981071926678621E-05</v>
@@ -9095,25 +9095,25 @@
         <v>9.962143853357243E-05</v>
       </c>
       <c r="T147" s="0">
-        <v>1020179.0999999996</v>
+        <v>1020179.1000000001</v>
       </c>
       <c r="U147" s="0">
-        <v>982186.0996527774</v>
+        <v>980941.4423076924</v>
       </c>
       <c r="V147" s="0">
-        <v>944193.0993055552</v>
+        <v>941703.7846153846</v>
       </c>
       <c r="W147" s="0">
-        <v>0.0004654874318393405</v>
+        <v>0.000498736534113579</v>
       </c>
       <c r="Z147" s="0">
-        <v>2989456.099999999</v>
+        <v>2989456.1</v>
       </c>
       <c r="AA147" s="0">
-        <v>2955947.1031249994</v>
+        <v>2955485.007954546</v>
       </c>
       <c r="AB147" s="0">
-        <v>2922438.1062499993</v>
+        <v>2921513.915909091</v>
       </c>
       <c r="AC147" s="0">
         <v>0.00013316465809974033</v>

</xml_diff>